<commit_message>
Small updates to documentation
* Add comparators to I2D2 in XLS dicitonary
* Correct PSU location in guidelines
</commit_message>
<xml_diff>
--- a/Support/A - Guides and Documentation/GLD_Dictionary_v01.xlsx
+++ b/Support/A - Guides and Documentation/GLD_Dictionary_v01.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb529026\Documents\gld\Support\Guides and Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb529026\Documents\gld\Support\A - Guides and Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF73109C-F8EF-42D1-A7A8-EDDCDD5B9241}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458D9869-6298-419C-A83B-6DC29AEB84D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C416022C-A35E-4942-8219-7CEF6CA35A15}"/>
   </bookViews>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="560">
   <si>
     <t>Module</t>
   </si>
@@ -2084,6 +2084,24 @@
   </si>
   <si>
     <t>Length of training in months, upper limit</t>
+  </si>
+  <si>
+    <t>psu</t>
+  </si>
+  <si>
+    <t>Primary Sampling unit</t>
+  </si>
+  <si>
+    <t>As in original survey, commonly string</t>
+  </si>
+  <si>
+    <t>ssu</t>
+  </si>
+  <si>
+    <t>Secondary Sampling unit</t>
+  </si>
+  <si>
+    <t>hhsize</t>
   </si>
 </sst>
 </file>
@@ -2392,9 +2410,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2565,6 +2580,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3147,27 +3165,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="22" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="65" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -3187,7 +3205,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="66"/>
+      <c r="A3" s="65"/>
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
@@ -3203,7 +3221,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="66"/>
+      <c r="A4" s="65"/>
       <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
@@ -3217,16 +3235,16 @@
         <v>17</v>
       </c>
       <c r="F4" s="2"/>
-      <c r="I4" s="67" t="s">
+      <c r="I4" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="67"/>
-      <c r="K4" s="67"/>
-      <c r="L4" s="67"/>
-      <c r="M4" s="67"/>
+      <c r="J4" s="66"/>
+      <c r="K4" s="66"/>
+      <c r="L4" s="66"/>
+      <c r="M4" s="66"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="66"/>
+      <c r="A5" s="65"/>
       <c r="B5" s="1" t="s">
         <v>19</v>
       </c>
@@ -3240,14 +3258,14 @@
         <v>19</v>
       </c>
       <c r="F5" s="2"/>
-      <c r="I5" s="67"/>
-      <c r="J5" s="67"/>
-      <c r="K5" s="67"/>
-      <c r="L5" s="67"/>
-      <c r="M5" s="67"/>
+      <c r="I5" s="66"/>
+      <c r="J5" s="66"/>
+      <c r="K5" s="66"/>
+      <c r="L5" s="66"/>
+      <c r="M5" s="66"/>
     </row>
     <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="66"/>
+      <c r="A6" s="65"/>
       <c r="B6" s="1" t="s">
         <v>22</v>
       </c>
@@ -3263,14 +3281,14 @@
       <c r="F6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="67"/>
-      <c r="J6" s="67"/>
-      <c r="K6" s="67"/>
-      <c r="L6" s="67"/>
-      <c r="M6" s="67"/>
+      <c r="I6" s="66"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="66"/>
+      <c r="L6" s="66"/>
+      <c r="M6" s="66"/>
     </row>
     <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="66"/>
+      <c r="A7" s="65"/>
       <c r="B7" s="1" t="s">
         <v>26</v>
       </c>
@@ -3288,7 +3306,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="66"/>
+      <c r="A8" s="65"/>
       <c r="B8" s="1" t="s">
         <v>30</v>
       </c>
@@ -3302,16 +3320,16 @@
         <v>32</v>
       </c>
       <c r="F8" s="2"/>
-      <c r="I8" s="67" t="s">
+      <c r="I8" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="J8" s="67"/>
-      <c r="K8" s="67"/>
-      <c r="L8" s="67"/>
-      <c r="M8" s="67"/>
+      <c r="J8" s="66"/>
+      <c r="K8" s="66"/>
+      <c r="L8" s="66"/>
+      <c r="M8" s="66"/>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="66"/>
+      <c r="A9" s="65"/>
       <c r="B9" s="1" t="s">
         <v>34</v>
       </c>
@@ -3325,14 +3343,14 @@
         <v>36</v>
       </c>
       <c r="F9" s="2"/>
-      <c r="I9" s="67"/>
-      <c r="J9" s="67"/>
-      <c r="K9" s="67"/>
-      <c r="L9" s="67"/>
-      <c r="M9" s="67"/>
+      <c r="I9" s="66"/>
+      <c r="J9" s="66"/>
+      <c r="K9" s="66"/>
+      <c r="L9" s="66"/>
+      <c r="M9" s="66"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="66"/>
+      <c r="A10" s="65"/>
       <c r="B10" s="1" t="s">
         <v>37</v>
       </c>
@@ -3346,14 +3364,14 @@
         <v>40</v>
       </c>
       <c r="F10" s="2"/>
-      <c r="I10" s="67"/>
-      <c r="J10" s="67"/>
-      <c r="K10" s="67"/>
-      <c r="L10" s="67"/>
-      <c r="M10" s="67"/>
+      <c r="I10" s="66"/>
+      <c r="J10" s="66"/>
+      <c r="K10" s="66"/>
+      <c r="L10" s="66"/>
+      <c r="M10" s="66"/>
     </row>
     <row r="11" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="66"/>
+      <c r="A11" s="65"/>
       <c r="B11" s="7" t="s">
         <v>41</v>
       </c>
@@ -3365,14 +3383,14 @@
       <c r="F11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I11" s="67"/>
-      <c r="J11" s="67"/>
-      <c r="K11" s="67"/>
-      <c r="L11" s="67"/>
-      <c r="M11" s="67"/>
+      <c r="I11" s="66"/>
+      <c r="J11" s="66"/>
+      <c r="K11" s="66"/>
+      <c r="L11" s="66"/>
+      <c r="M11" s="66"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="66"/>
+      <c r="A12" s="65"/>
       <c r="B12" s="1" t="s">
         <v>44</v>
       </c>
@@ -3388,7 +3406,7 @@
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="66"/>
+      <c r="A13" s="65"/>
       <c r="B13" s="1" t="s">
         <v>47</v>
       </c>
@@ -3424,7 +3442,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="65" t="s">
+      <c r="A15" s="64" t="s">
         <v>50</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -3442,7 +3460,7 @@
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="65"/>
+      <c r="A16" s="64"/>
       <c r="B16" s="4" t="s">
         <v>55</v>
       </c>
@@ -3460,7 +3478,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="65"/>
+      <c r="A17" s="64"/>
       <c r="B17" s="4" t="s">
         <v>60</v>
       </c>
@@ -3474,16 +3492,16 @@
       <c r="F17" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="I17" s="67" t="s">
+      <c r="I17" s="66" t="s">
         <v>63</v>
       </c>
-      <c r="J17" s="67"/>
-      <c r="K17" s="67"/>
-      <c r="L17" s="67"/>
-      <c r="M17" s="67"/>
+      <c r="J17" s="66"/>
+      <c r="K17" s="66"/>
+      <c r="L17" s="66"/>
+      <c r="M17" s="66"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="65"/>
+      <c r="A18" s="64"/>
       <c r="B18" s="4" t="s">
         <v>64</v>
       </c>
@@ -3499,7 +3517,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="65"/>
+      <c r="A19" s="64"/>
       <c r="B19" s="4" t="s">
         <v>67</v>
       </c>
@@ -3515,7 +3533,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="69" t="s">
+      <c r="A20" s="68" t="s">
         <v>70</v>
       </c>
       <c r="B20" s="13" t="s">
@@ -3533,16 +3551,16 @@
       <c r="F20" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="I20" s="70" t="s">
+      <c r="I20" s="69" t="s">
         <v>71</v>
       </c>
-      <c r="J20" s="71"/>
-      <c r="K20" s="71"/>
-      <c r="L20" s="71"/>
-      <c r="M20" s="71"/>
+      <c r="J20" s="70"/>
+      <c r="K20" s="70"/>
+      <c r="L20" s="70"/>
+      <c r="M20" s="70"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="69"/>
+      <c r="A21" s="68"/>
       <c r="B21" s="13" t="s">
         <v>49</v>
       </c>
@@ -3558,14 +3576,14 @@
       <c r="F21" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="I21" s="71"/>
-      <c r="J21" s="71"/>
-      <c r="K21" s="71"/>
-      <c r="L21" s="71"/>
-      <c r="M21" s="71"/>
+      <c r="I21" s="70"/>
+      <c r="J21" s="70"/>
+      <c r="K21" s="70"/>
+      <c r="L21" s="70"/>
+      <c r="M21" s="70"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="66" t="s">
+      <c r="A22" s="65" t="s">
         <v>72</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -3581,14 +3599,14 @@
         <v>73</v>
       </c>
       <c r="F22" s="2"/>
-      <c r="I22" s="71"/>
-      <c r="J22" s="71"/>
-      <c r="K22" s="71"/>
-      <c r="L22" s="71"/>
-      <c r="M22" s="71"/>
+      <c r="I22" s="70"/>
+      <c r="J22" s="70"/>
+      <c r="K22" s="70"/>
+      <c r="L22" s="70"/>
+      <c r="M22" s="70"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="66"/>
+      <c r="A23" s="65"/>
       <c r="B23" s="1" t="s">
         <v>75</v>
       </c>
@@ -3602,14 +3620,14 @@
         <v>78</v>
       </c>
       <c r="F23" s="2"/>
-      <c r="I23" s="71"/>
-      <c r="J23" s="71"/>
-      <c r="K23" s="71"/>
-      <c r="L23" s="71"/>
-      <c r="M23" s="71"/>
+      <c r="I23" s="70"/>
+      <c r="J23" s="70"/>
+      <c r="K23" s="70"/>
+      <c r="L23" s="70"/>
+      <c r="M23" s="70"/>
     </row>
     <row r="24" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="66"/>
+      <c r="A24" s="65"/>
       <c r="B24" s="1" t="s">
         <v>79</v>
       </c>
@@ -3625,14 +3643,14 @@
       <c r="F24" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="I24" s="71"/>
-      <c r="J24" s="71"/>
-      <c r="K24" s="71"/>
-      <c r="L24" s="71"/>
-      <c r="M24" s="71"/>
+      <c r="I24" s="70"/>
+      <c r="J24" s="70"/>
+      <c r="K24" s="70"/>
+      <c r="L24" s="70"/>
+      <c r="M24" s="70"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="66"/>
+      <c r="A25" s="65"/>
       <c r="B25" s="1" t="s">
         <v>84</v>
       </c>
@@ -3648,7 +3666,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="66"/>
+      <c r="A26" s="65"/>
       <c r="B26" s="1" t="s">
         <v>88</v>
       </c>
@@ -3664,7 +3682,7 @@
       <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="66"/>
+      <c r="A27" s="65"/>
       <c r="B27" s="1" t="s">
         <v>91</v>
       </c>
@@ -3675,12 +3693,12 @@
         <v>93</v>
       </c>
       <c r="E27" s="6"/>
-      <c r="F27" s="68" t="s">
+      <c r="F27" s="67" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="66"/>
+      <c r="A28" s="65"/>
       <c r="B28" s="1" t="s">
         <v>95</v>
       </c>
@@ -3691,10 +3709,10 @@
         <v>93</v>
       </c>
       <c r="E28" s="6"/>
-      <c r="F28" s="68"/>
+      <c r="F28" s="67"/>
     </row>
     <row r="29" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="66"/>
+      <c r="A29" s="65"/>
       <c r="B29" s="1" t="s">
         <v>97</v>
       </c>
@@ -3705,10 +3723,10 @@
         <v>93</v>
       </c>
       <c r="E29" s="6"/>
-      <c r="F29" s="68"/>
+      <c r="F29" s="67"/>
     </row>
     <row r="30" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="66"/>
+      <c r="A30" s="65"/>
       <c r="B30" s="1" t="s">
         <v>99</v>
       </c>
@@ -3719,10 +3737,10 @@
         <v>93</v>
       </c>
       <c r="E30" s="6"/>
-      <c r="F30" s="68"/>
+      <c r="F30" s="67"/>
     </row>
     <row r="31" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="66"/>
+      <c r="A31" s="65"/>
       <c r="B31" s="1" t="s">
         <v>101</v>
       </c>
@@ -3733,10 +3751,10 @@
         <v>93</v>
       </c>
       <c r="E31" s="6"/>
-      <c r="F31" s="68"/>
+      <c r="F31" s="67"/>
     </row>
     <row r="32" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="66"/>
+      <c r="A32" s="65"/>
       <c r="B32" s="1" t="s">
         <v>103</v>
       </c>
@@ -3747,10 +3765,10 @@
         <v>93</v>
       </c>
       <c r="E32" s="6"/>
-      <c r="F32" s="68"/>
+      <c r="F32" s="67"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="65" t="s">
+      <c r="A33" s="64" t="s">
         <v>105</v>
       </c>
       <c r="B33" s="4" t="s">
@@ -3768,7 +3786,7 @@
       <c r="F33" s="5"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="65"/>
+      <c r="A34" s="64"/>
       <c r="B34" s="4" t="s">
         <v>110</v>
       </c>
@@ -3784,7 +3802,7 @@
       <c r="F34" s="5"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="65"/>
+      <c r="A35" s="64"/>
       <c r="B35" s="4" t="s">
         <v>112</v>
       </c>
@@ -3800,7 +3818,7 @@
       <c r="F35" s="5"/>
     </row>
     <row r="36" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A36" s="65"/>
+      <c r="A36" s="64"/>
       <c r="B36" s="4" t="s">
         <v>115</v>
       </c>
@@ -3816,7 +3834,7 @@
       <c r="F36" s="5"/>
     </row>
     <row r="37" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A37" s="65"/>
+      <c r="A37" s="64"/>
       <c r="B37" s="4" t="s">
         <v>119</v>
       </c>
@@ -3832,7 +3850,7 @@
       <c r="F37" s="5"/>
     </row>
     <row r="38" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A38" s="65"/>
+      <c r="A38" s="64"/>
       <c r="B38" s="4" t="s">
         <v>123</v>
       </c>
@@ -3848,7 +3866,7 @@
       <c r="F38" s="5"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="66" t="s">
+      <c r="A39" s="65" t="s">
         <v>127</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -3866,7 +3884,7 @@
       <c r="F39" s="2"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="66"/>
+      <c r="A40" s="65"/>
       <c r="B40" s="1" t="s">
         <v>131</v>
       </c>
@@ -3882,7 +3900,7 @@
       <c r="F40" s="2"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="66"/>
+      <c r="A41" s="65"/>
       <c r="B41" s="1" t="s">
         <v>134</v>
       </c>
@@ -3898,7 +3916,7 @@
       <c r="F41" s="2"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="66"/>
+      <c r="A42" s="65"/>
       <c r="B42" s="1" t="s">
         <v>137</v>
       </c>
@@ -3914,7 +3932,7 @@
       <c r="F42" s="2"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="66"/>
+      <c r="A43" s="65"/>
       <c r="B43" s="1" t="s">
         <v>139</v>
       </c>
@@ -3930,7 +3948,7 @@
       <c r="F43" s="2"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="66"/>
+      <c r="A44" s="65"/>
       <c r="B44" s="1" t="s">
         <v>141</v>
       </c>
@@ -3946,7 +3964,7 @@
       <c r="F44" s="2"/>
     </row>
     <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="66"/>
+      <c r="A45" s="65"/>
       <c r="B45" s="1" t="s">
         <v>144</v>
       </c>
@@ -3964,7 +3982,7 @@
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="66"/>
+      <c r="A46" s="65"/>
       <c r="B46" s="1" t="s">
         <v>148</v>
       </c>
@@ -3980,7 +3998,7 @@
       <c r="F46" s="2"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="66"/>
+      <c r="A47" s="65"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -3988,7 +4006,7 @@
       <c r="F47" s="2"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="66"/>
+      <c r="A48" s="65"/>
       <c r="B48" s="1" t="s">
         <v>150</v>
       </c>
@@ -4004,7 +4022,7 @@
       <c r="F48" s="2"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="66"/>
+      <c r="A49" s="65"/>
       <c r="B49" s="1" t="s">
         <v>154</v>
       </c>
@@ -4020,7 +4038,7 @@
       <c r="F49" s="2"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="66"/>
+      <c r="A50" s="65"/>
       <c r="B50" s="1" t="s">
         <v>158</v>
       </c>
@@ -4036,7 +4054,7 @@
       <c r="F50" s="2"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="66"/>
+      <c r="A51" s="65"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -4044,7 +4062,7 @@
       <c r="F51" s="2"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="66"/>
+      <c r="A52" s="65"/>
       <c r="B52" s="1" t="s">
         <v>160</v>
       </c>
@@ -4060,7 +4078,7 @@
       <c r="F52" s="2"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="66"/>
+      <c r="A53" s="65"/>
       <c r="B53" s="1" t="s">
         <v>163</v>
       </c>
@@ -4076,7 +4094,7 @@
       <c r="F53" s="2"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="66"/>
+      <c r="A54" s="65"/>
       <c r="B54" s="1" t="s">
         <v>166</v>
       </c>
@@ -4092,7 +4110,7 @@
       <c r="F54" s="2"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="66"/>
+      <c r="A55" s="65"/>
       <c r="B55" s="1" t="s">
         <v>169</v>
       </c>
@@ -4108,7 +4126,7 @@
       <c r="F55" s="2"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="66"/>
+      <c r="A56" s="65"/>
       <c r="B56" s="1" t="s">
         <v>171</v>
       </c>
@@ -4122,7 +4140,7 @@
       <c r="F56" s="2"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="66"/>
+      <c r="A57" s="65"/>
       <c r="B57" s="1" t="s">
         <v>173</v>
       </c>
@@ -4136,7 +4154,7 @@
       <c r="F57" s="2"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="66"/>
+      <c r="A58" s="65"/>
       <c r="B58" s="1" t="s">
         <v>175</v>
       </c>
@@ -4152,7 +4170,7 @@
       <c r="F58" s="2"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="66"/>
+      <c r="A59" s="65"/>
       <c r="B59" s="1" t="s">
         <v>178</v>
       </c>
@@ -4168,7 +4186,7 @@
       <c r="F59" s="2"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="66"/>
+      <c r="A60" s="65"/>
       <c r="B60" s="1" t="s">
         <v>180</v>
       </c>
@@ -4184,7 +4202,7 @@
       <c r="F60" s="2"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="66"/>
+      <c r="A61" s="65"/>
       <c r="B61" s="1" t="s">
         <v>182</v>
       </c>
@@ -4200,7 +4218,7 @@
       <c r="F61" s="2"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="66"/>
+      <c r="A62" s="65"/>
       <c r="B62" s="1" t="s">
         <v>184</v>
       </c>
@@ -4216,7 +4234,7 @@
       <c r="F62" s="2"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="66"/>
+      <c r="A63" s="65"/>
       <c r="B63" s="1" t="s">
         <v>186</v>
       </c>
@@ -4232,7 +4250,7 @@
       <c r="F63" s="2"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="66"/>
+      <c r="A64" s="65"/>
       <c r="B64" s="1" t="s">
         <v>188</v>
       </c>
@@ -4248,7 +4266,7 @@
       <c r="F64" s="2"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="66"/>
+      <c r="A65" s="65"/>
       <c r="B65" s="1" t="s">
         <v>190</v>
       </c>
@@ -4262,7 +4280,7 @@
       <c r="F65" s="2"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="66"/>
+      <c r="A66" s="65"/>
       <c r="B66" s="1" t="s">
         <v>193</v>
       </c>
@@ -4278,7 +4296,7 @@
       <c r="F66" s="2"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="66"/>
+      <c r="A67" s="65"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
@@ -4286,7 +4304,7 @@
       <c r="F67" s="2"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="66"/>
+      <c r="A68" s="65"/>
       <c r="B68" s="1" t="s">
         <v>195</v>
       </c>
@@ -4302,7 +4320,7 @@
       <c r="F68" s="2"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="66"/>
+      <c r="A69" s="65"/>
       <c r="B69" s="1" t="s">
         <v>198</v>
       </c>
@@ -4318,7 +4336,7 @@
       <c r="F69" s="2"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="66"/>
+      <c r="A70" s="65"/>
       <c r="B70" s="1" t="s">
         <v>201</v>
       </c>
@@ -4332,7 +4350,7 @@
       <c r="F70" s="2"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="66"/>
+      <c r="A71" s="65"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
@@ -4340,7 +4358,7 @@
       <c r="F71" s="2"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="66"/>
+      <c r="A72" s="65"/>
       <c r="B72" s="1" t="s">
         <v>203</v>
       </c>
@@ -4356,7 +4374,7 @@
       <c r="F72" s="2"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="66"/>
+      <c r="A73" s="65"/>
       <c r="B73" s="1" t="s">
         <v>205</v>
       </c>
@@ -4372,7 +4390,7 @@
       <c r="F73" s="2"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="66"/>
+      <c r="A74" s="65"/>
       <c r="B74" s="1" t="s">
         <v>208</v>
       </c>
@@ -4388,7 +4406,7 @@
       <c r="F74" s="2"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="66"/>
+      <c r="A75" s="65"/>
       <c r="B75" s="1" t="s">
         <v>210</v>
       </c>
@@ -4402,7 +4420,7 @@
       <c r="F75" s="2"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="66"/>
+      <c r="A76" s="65"/>
       <c r="B76" s="1" t="s">
         <v>212</v>
       </c>
@@ -4416,7 +4434,7 @@
       <c r="F76" s="2"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="66"/>
+      <c r="A77" s="65"/>
       <c r="B77" s="1" t="s">
         <v>214</v>
       </c>
@@ -4430,7 +4448,7 @@
       <c r="F77" s="2"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="66"/>
+      <c r="A78" s="65"/>
       <c r="B78" s="1" t="s">
         <v>216</v>
       </c>
@@ -4444,7 +4462,7 @@
       <c r="F78" s="2"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="66"/>
+      <c r="A79" s="65"/>
       <c r="B79" s="1" t="s">
         <v>218</v>
       </c>
@@ -4458,7 +4476,7 @@
       <c r="F79" s="2"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="66"/>
+      <c r="A80" s="65"/>
       <c r="B80" s="1" t="s">
         <v>220</v>
       </c>
@@ -4472,7 +4490,7 @@
       <c r="F80" s="2"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="66"/>
+      <c r="A81" s="65"/>
       <c r="B81" s="1" t="s">
         <v>222</v>
       </c>
@@ -4486,7 +4504,7 @@
       <c r="F81" s="2"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="66"/>
+      <c r="A82" s="65"/>
       <c r="B82" s="1" t="s">
         <v>224</v>
       </c>
@@ -4500,7 +4518,7 @@
       <c r="F82" s="2"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="66"/>
+      <c r="A83" s="65"/>
       <c r="B83" s="1" t="s">
         <v>226</v>
       </c>
@@ -4514,7 +4532,7 @@
       <c r="F83" s="2"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="66"/>
+      <c r="A84" s="65"/>
       <c r="B84" s="1" t="s">
         <v>228</v>
       </c>
@@ -4528,7 +4546,7 @@
       <c r="F84" s="2"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="66"/>
+      <c r="A85" s="65"/>
       <c r="B85" s="1" t="s">
         <v>230</v>
       </c>
@@ -4542,7 +4560,7 @@
       <c r="F85" s="2"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="66"/>
+      <c r="A86" s="65"/>
       <c r="B86" s="1" t="s">
         <v>232</v>
       </c>
@@ -4558,7 +4576,7 @@
       <c r="F86" s="2"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="66"/>
+      <c r="A87" s="65"/>
       <c r="B87" s="1" t="s">
         <v>234</v>
       </c>
@@ -4572,7 +4590,7 @@
       <c r="F87" s="2"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="66"/>
+      <c r="A88" s="65"/>
       <c r="B88" s="1" t="s">
         <v>236</v>
       </c>
@@ -4586,7 +4604,7 @@
       <c r="F88" s="2"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="66"/>
+      <c r="A89" s="65"/>
       <c r="B89" s="1" t="s">
         <v>238</v>
       </c>
@@ -4600,7 +4618,7 @@
       <c r="F89" s="2"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="66"/>
+      <c r="A90" s="65"/>
       <c r="B90" s="1" t="s">
         <v>240</v>
       </c>
@@ -4616,7 +4634,7 @@
       <c r="F90" s="2"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="66"/>
+      <c r="A91" s="65"/>
       <c r="B91" s="1" t="s">
         <v>242</v>
       </c>
@@ -4630,7 +4648,7 @@
       <c r="F91" s="2"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="66"/>
+      <c r="A92" s="65"/>
       <c r="B92" s="1" t="s">
         <v>244</v>
       </c>
@@ -4644,7 +4662,7 @@
       <c r="F92" s="2"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="66"/>
+      <c r="A93" s="65"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
@@ -4652,7 +4670,7 @@
       <c r="F93" s="2"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="66"/>
+      <c r="A94" s="65"/>
       <c r="B94" s="1" t="s">
         <v>246</v>
       </c>
@@ -4666,7 +4684,7 @@
       <c r="F94" s="2"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="66"/>
+      <c r="A95" s="65"/>
       <c r="B95" s="1" t="s">
         <v>248</v>
       </c>
@@ -4680,7 +4698,7 @@
       <c r="F95" s="2"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="66"/>
+      <c r="A96" s="65"/>
       <c r="B96" s="1" t="s">
         <v>250</v>
       </c>
@@ -4694,7 +4712,7 @@
       <c r="F96" s="2"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="66"/>
+      <c r="A97" s="65"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
@@ -4702,7 +4720,7 @@
       <c r="F97" s="2"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="66"/>
+      <c r="A98" s="65"/>
       <c r="B98" s="1" t="s">
         <v>252</v>
       </c>
@@ -4716,7 +4734,7 @@
       <c r="F98" s="2"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="66"/>
+      <c r="A99" s="65"/>
       <c r="B99" s="1" t="s">
         <v>254</v>
       </c>
@@ -4730,7 +4748,7 @@
       <c r="F99" s="2"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="66"/>
+      <c r="A100" s="65"/>
       <c r="B100" s="1" t="s">
         <v>257</v>
       </c>
@@ -4744,7 +4762,7 @@
       <c r="F100" s="2"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="66"/>
+      <c r="A101" s="65"/>
       <c r="B101" s="1" t="s">
         <v>259</v>
       </c>
@@ -4758,7 +4776,7 @@
       <c r="F101" s="2"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="66"/>
+      <c r="A102" s="65"/>
       <c r="B102" s="1" t="s">
         <v>262</v>
       </c>
@@ -4772,7 +4790,7 @@
       <c r="F102" s="2"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="66"/>
+      <c r="A103" s="65"/>
       <c r="B103" s="1" t="s">
         <v>264</v>
       </c>
@@ -4786,7 +4804,7 @@
       <c r="F103" s="2"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="66"/>
+      <c r="A104" s="65"/>
       <c r="B104" s="1" t="s">
         <v>266</v>
       </c>
@@ -4800,7 +4818,7 @@
       <c r="F104" s="2"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="66"/>
+      <c r="A105" s="65"/>
       <c r="B105" s="1" t="s">
         <v>268</v>
       </c>
@@ -4814,7 +4832,7 @@
       <c r="F105" s="2"/>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="66"/>
+      <c r="A106" s="65"/>
       <c r="B106" s="1" t="s">
         <v>270</v>
       </c>
@@ -4828,7 +4846,7 @@
       <c r="F106" s="2"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" s="66"/>
+      <c r="A107" s="65"/>
       <c r="B107" s="1" t="s">
         <v>272</v>
       </c>
@@ -4842,7 +4860,7 @@
       <c r="F107" s="2"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" s="66"/>
+      <c r="A108" s="65"/>
       <c r="B108" s="1" t="s">
         <v>274</v>
       </c>
@@ -4856,7 +4874,7 @@
       <c r="F108" s="2"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" s="66"/>
+      <c r="A109" s="65"/>
       <c r="B109" s="1" t="s">
         <v>276</v>
       </c>
@@ -4870,7 +4888,7 @@
       <c r="F109" s="2"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A110" s="66"/>
+      <c r="A110" s="65"/>
       <c r="B110" s="1" t="s">
         <v>278</v>
       </c>
@@ -4886,7 +4904,7 @@
       <c r="F110" s="2"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" s="66"/>
+      <c r="A111" s="65"/>
       <c r="B111" s="1" t="s">
         <v>280</v>
       </c>
@@ -4900,7 +4918,7 @@
       <c r="F111" s="2"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A112" s="66"/>
+      <c r="A112" s="65"/>
       <c r="B112" s="1" t="s">
         <v>282</v>
       </c>
@@ -4914,7 +4932,7 @@
       <c r="F112" s="2"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" s="66"/>
+      <c r="A113" s="65"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
@@ -4922,7 +4940,7 @@
       <c r="F113" s="2"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A114" s="66"/>
+      <c r="A114" s="65"/>
       <c r="B114" s="1" t="s">
         <v>284</v>
       </c>
@@ -4936,7 +4954,7 @@
       <c r="F114" s="2"/>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A115" s="66"/>
+      <c r="A115" s="65"/>
       <c r="B115" s="1" t="s">
         <v>287</v>
       </c>
@@ -4950,7 +4968,7 @@
       <c r="F115" s="2"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A116" s="66"/>
+      <c r="A116" s="65"/>
       <c r="B116" s="1" t="s">
         <v>289</v>
       </c>
@@ -4964,7 +4982,7 @@
       <c r="F116" s="2"/>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A117" s="66"/>
+      <c r="A117" s="65"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
@@ -4972,7 +4990,7 @@
       <c r="F117" s="2"/>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A118" s="66"/>
+      <c r="A118" s="65"/>
       <c r="B118" s="1" t="s">
         <v>291</v>
       </c>
@@ -4986,7 +5004,7 @@
       <c r="F118" s="2"/>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A119" s="66"/>
+      <c r="A119" s="65"/>
       <c r="B119" s="1" t="s">
         <v>293</v>
       </c>
@@ -5000,7 +5018,7 @@
       <c r="F119" s="2"/>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A120" s="66"/>
+      <c r="A120" s="65"/>
       <c r="B120" s="1" t="s">
         <v>296</v>
       </c>
@@ -5014,7 +5032,7 @@
       <c r="F120" s="2"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121" s="66"/>
+      <c r="A121" s="65"/>
       <c r="B121" s="1" t="s">
         <v>298</v>
       </c>
@@ -5028,7 +5046,7 @@
       <c r="F121" s="2"/>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A122" s="66"/>
+      <c r="A122" s="65"/>
       <c r="B122" s="1" t="s">
         <v>301</v>
       </c>
@@ -5042,7 +5060,7 @@
       <c r="F122" s="2"/>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A123" s="66"/>
+      <c r="A123" s="65"/>
       <c r="B123" s="1" t="s">
         <v>303</v>
       </c>
@@ -5054,7 +5072,7 @@
       <c r="F123" s="2"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A124" s="66"/>
+      <c r="A124" s="65"/>
       <c r="B124" s="1" t="s">
         <v>305</v>
       </c>
@@ -5068,7 +5086,7 @@
       <c r="F124" s="2"/>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A125" s="66"/>
+      <c r="A125" s="65"/>
       <c r="B125" s="1" t="s">
         <v>307</v>
       </c>
@@ -5082,7 +5100,7 @@
       <c r="F125" s="2"/>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A126" s="66"/>
+      <c r="A126" s="65"/>
       <c r="B126" s="1" t="s">
         <v>309</v>
       </c>
@@ -5096,7 +5114,7 @@
       <c r="F126" s="2"/>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A127" s="66"/>
+      <c r="A127" s="65"/>
       <c r="B127" s="1" t="s">
         <v>311</v>
       </c>
@@ -5110,7 +5128,7 @@
       <c r="F127" s="2"/>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A128" s="66"/>
+      <c r="A128" s="65"/>
       <c r="B128" s="1" t="s">
         <v>313</v>
       </c>
@@ -5126,7 +5144,7 @@
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A129" s="66"/>
+      <c r="A129" s="65"/>
       <c r="B129" s="1" t="s">
         <v>315</v>
       </c>
@@ -5140,7 +5158,7 @@
       <c r="F129" s="2"/>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A130" s="66"/>
+      <c r="A130" s="65"/>
       <c r="B130" s="1" t="s">
         <v>317</v>
       </c>
@@ -5154,7 +5172,7 @@
       <c r="F130" s="2"/>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A131" s="66"/>
+      <c r="A131" s="65"/>
       <c r="B131" s="1" t="s">
         <v>319</v>
       </c>
@@ -5168,7 +5186,7 @@
       <c r="F131" s="2"/>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A132" s="66"/>
+      <c r="A132" s="65"/>
       <c r="B132" s="1" t="s">
         <v>321</v>
       </c>
@@ -5184,7 +5202,7 @@
       <c r="F132" s="2"/>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A133" s="66"/>
+      <c r="A133" s="65"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
       <c r="D133" s="1"/>
@@ -5194,7 +5212,7 @@
       <c r="F133" s="2"/>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A134" s="66"/>
+      <c r="A134" s="65"/>
       <c r="B134" s="1" t="s">
         <v>324</v>
       </c>
@@ -5208,7 +5226,7 @@
       <c r="F134" s="2"/>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A135" s="66"/>
+      <c r="A135" s="65"/>
       <c r="B135" s="1" t="s">
         <v>326</v>
       </c>
@@ -5222,7 +5240,7 @@
       <c r="F135" s="2"/>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A136" s="66"/>
+      <c r="A136" s="65"/>
       <c r="B136" s="1" t="s">
         <v>328</v>
       </c>
@@ -5260,8 +5278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8655A41D-FAAE-4875-A0C4-A516EEA673B9}">
   <dimension ref="A1:F168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5275,27 +5293,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="22" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="71" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="18" t="s">
@@ -5313,7 +5331,7 @@
       <c r="F2" s="20"/>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="72"/>
+      <c r="A3" s="71"/>
       <c r="B3" s="15" t="s">
         <v>7</v>
       </c>
@@ -5331,7 +5349,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="72"/>
+      <c r="A4" s="71"/>
       <c r="B4" s="18" t="s">
         <v>12</v>
       </c>
@@ -5347,7 +5365,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="72"/>
+      <c r="A5" s="71"/>
       <c r="B5" s="18" t="s">
         <v>466</v>
       </c>
@@ -5363,7 +5381,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="72"/>
+      <c r="A6" s="71"/>
       <c r="B6" s="18" t="s">
         <v>537</v>
       </c>
@@ -5377,7 +5395,7 @@
       <c r="F6" s="20"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="72"/>
+      <c r="A7" s="71"/>
       <c r="B7" s="18" t="s">
         <v>538</v>
       </c>
@@ -5391,7 +5409,7 @@
       <c r="F7" s="20"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="72"/>
+      <c r="A8" s="71"/>
       <c r="B8" s="18" t="s">
         <v>539</v>
       </c>
@@ -5405,7 +5423,7 @@
       <c r="F8" s="20"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="72"/>
+      <c r="A9" s="71"/>
       <c r="B9" s="18" t="s">
         <v>19</v>
       </c>
@@ -5421,7 +5439,7 @@
       <c r="F9" s="20"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="72"/>
+      <c r="A10" s="71"/>
       <c r="B10" s="18" t="s">
         <v>432</v>
       </c>
@@ -5435,7 +5453,7 @@
       <c r="F10" s="20"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="72"/>
+      <c r="A11" s="71"/>
       <c r="B11" s="18" t="s">
         <v>433</v>
       </c>
@@ -5449,7 +5467,7 @@
       <c r="F11" s="20"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="72"/>
+      <c r="A12" s="71"/>
       <c r="B12" s="18" t="s">
         <v>434</v>
       </c>
@@ -5463,7 +5481,7 @@
       <c r="F12" s="20"/>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="72"/>
+      <c r="A13" s="71"/>
       <c r="B13" s="18" t="s">
         <v>22</v>
       </c>
@@ -5481,7 +5499,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="72"/>
+      <c r="A14" s="71"/>
       <c r="B14" s="18" t="s">
         <v>26</v>
       </c>
@@ -5499,7 +5517,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="72"/>
+      <c r="A15" s="71"/>
       <c r="B15" s="18" t="s">
         <v>30</v>
       </c>
@@ -5515,7 +5533,7 @@
       <c r="F15" s="20"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="72"/>
+      <c r="A16" s="71"/>
       <c r="B16" s="18" t="s">
         <v>34</v>
       </c>
@@ -5531,7 +5549,7 @@
       <c r="F16" s="20"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="72"/>
+      <c r="A17" s="71"/>
       <c r="B17" s="18" t="s">
         <v>37</v>
       </c>
@@ -5546,150 +5564,152 @@
       </c>
       <c r="F17" s="20"/>
     </row>
-    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="72"/>
-      <c r="B18" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="20" t="s">
-        <v>43</v>
-      </c>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="71"/>
+      <c r="B18" s="78" t="s">
+        <v>554</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>555</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>556</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>554</v>
+      </c>
+      <c r="F18" s="20"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="72"/>
-      <c r="B19" s="18" t="s">
-        <v>430</v>
+      <c r="A19" s="71"/>
+      <c r="B19" s="78" t="s">
+        <v>557</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>431</v>
+        <v>558</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>9</v>
+        <v>556</v>
       </c>
       <c r="E19" s="19"/>
       <c r="F19" s="20"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="73" t="s">
+      <c r="A20" s="71"/>
+      <c r="B20" s="18" t="s">
+        <v>430</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>431</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="19"/>
+      <c r="F20" s="20"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="72" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="B21" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="C21" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="34" t="s">
+      <c r="D21" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="36" t="s">
+      <c r="E21" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="F20" s="35"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="73"/>
-      <c r="B21" s="38" t="s">
+      <c r="F21" s="34"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="72"/>
+      <c r="B22" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="38" t="s">
+      <c r="C22" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="D21" s="38" t="s">
+      <c r="D22" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="E21" s="40" t="s">
+      <c r="E22" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="F21" s="39" t="s">
+      <c r="F22" s="38" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="73"/>
-      <c r="B22" s="38" t="s">
+    <row r="23" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="72"/>
+      <c r="B23" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="38" t="s">
+      <c r="C23" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="D22" s="38" t="s">
+      <c r="D23" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="40"/>
-      <c r="F22" s="39" t="s">
+      <c r="E23" s="39"/>
+      <c r="F23" s="38" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="73"/>
-      <c r="B23" s="38" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="72"/>
+      <c r="B24" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="C23" s="38" t="s">
+      <c r="C24" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="D23" s="38" t="s">
+      <c r="D24" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="E23" s="40"/>
-      <c r="F23" s="39" t="s">
+      <c r="E24" s="39"/>
+      <c r="F24" s="38" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="73"/>
-      <c r="B24" s="46" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="46" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" s="46" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="72"/>
+      <c r="B25" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="50" t="s">
-        <v>46</v>
-      </c>
-      <c r="F24" s="47"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="73"/>
-      <c r="B25" s="46" t="s">
+      <c r="E25" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="46" t="s">
-        <v>48</v>
-      </c>
-      <c r="D25" s="46" t="s">
+      <c r="F25" s="46"/>
+    </row>
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="72"/>
+      <c r="B26" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="50" t="s">
-        <v>47</v>
-      </c>
-      <c r="F25" s="47"/>
-    </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="73"/>
-      <c r="B26" s="42" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" s="42" t="s">
-        <v>68</v>
-      </c>
-      <c r="D26" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="44"/>
-      <c r="F26" s="43" t="s">
+      <c r="E26" s="43"/>
+      <c r="F26" s="42" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="77" t="s">
+      <c r="A27" s="76" t="s">
         <v>72</v>
       </c>
       <c r="B27" s="18" t="s">
@@ -5701,11 +5721,13 @@
       <c r="D27" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="E27" s="19"/>
+      <c r="E27" s="19" t="s">
+        <v>559</v>
+      </c>
       <c r="F27" s="20"/>
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="77"/>
+      <c r="A28" s="76"/>
       <c r="B28" s="18" t="s">
         <v>73</v>
       </c>
@@ -5721,7 +5743,7 @@
       <c r="F28" s="20"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="77"/>
+      <c r="A29" s="76"/>
       <c r="B29" s="18" t="s">
         <v>75</v>
       </c>
@@ -5737,7 +5759,7 @@
       <c r="F29" s="20"/>
     </row>
     <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="77"/>
+      <c r="A30" s="76"/>
       <c r="B30" s="18" t="s">
         <v>79</v>
       </c>
@@ -5755,7 +5777,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="77"/>
+      <c r="A31" s="76"/>
       <c r="B31" s="18" t="s">
         <v>84</v>
       </c>
@@ -5771,7 +5793,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="77"/>
+      <c r="A32" s="76"/>
       <c r="B32" s="18" t="s">
         <v>88</v>
       </c>
@@ -5787,7 +5809,7 @@
       <c r="F32" s="20"/>
     </row>
     <row r="33" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="77"/>
+      <c r="A33" s="76"/>
       <c r="B33" s="18" t="s">
         <v>91</v>
       </c>
@@ -5798,12 +5820,12 @@
         <v>93</v>
       </c>
       <c r="E33" s="19"/>
-      <c r="F33" s="74" t="s">
+      <c r="F33" s="73" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="77"/>
+      <c r="A34" s="76"/>
       <c r="B34" s="18" t="s">
         <v>95</v>
       </c>
@@ -5814,10 +5836,10 @@
         <v>93</v>
       </c>
       <c r="E34" s="19"/>
-      <c r="F34" s="75"/>
+      <c r="F34" s="74"/>
     </row>
     <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="77"/>
+      <c r="A35" s="76"/>
       <c r="B35" s="18" t="s">
         <v>97</v>
       </c>
@@ -5828,10 +5850,10 @@
         <v>93</v>
       </c>
       <c r="E35" s="19"/>
-      <c r="F35" s="75"/>
+      <c r="F35" s="74"/>
     </row>
     <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="77"/>
+      <c r="A36" s="76"/>
       <c r="B36" s="18" t="s">
         <v>99</v>
       </c>
@@ -5842,10 +5864,10 @@
         <v>93</v>
       </c>
       <c r="E36" s="19"/>
-      <c r="F36" s="75"/>
+      <c r="F36" s="74"/>
     </row>
     <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="77"/>
+      <c r="A37" s="76"/>
       <c r="B37" s="18" t="s">
         <v>101</v>
       </c>
@@ -5856,10 +5878,10 @@
         <v>93</v>
       </c>
       <c r="E37" s="19"/>
-      <c r="F37" s="75"/>
+      <c r="F37" s="74"/>
     </row>
     <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="77"/>
+      <c r="A38" s="76"/>
       <c r="B38" s="18" t="s">
         <v>103</v>
       </c>
@@ -5870,262 +5892,262 @@
         <v>93</v>
       </c>
       <c r="E38" s="19"/>
-      <c r="F38" s="76"/>
+      <c r="F38" s="75"/>
     </row>
     <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="78" t="s">
+      <c r="A39" s="77" t="s">
         <v>484</v>
       </c>
-      <c r="B39" s="34" t="s">
+      <c r="B39" s="33" t="s">
         <v>486</v>
       </c>
-      <c r="C39" s="35" t="s">
+      <c r="C39" s="34" t="s">
         <v>487</v>
       </c>
-      <c r="D39" s="35" t="s">
+      <c r="D39" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="E39" s="36"/>
-      <c r="F39" s="37"/>
+      <c r="E39" s="35"/>
+      <c r="F39" s="36"/>
     </row>
     <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="78"/>
-      <c r="B40" s="48" t="s">
+      <c r="A40" s="77"/>
+      <c r="B40" s="47" t="s">
         <v>489</v>
       </c>
-      <c r="C40" s="49" t="s">
+      <c r="C40" s="48" t="s">
         <v>490</v>
       </c>
-      <c r="D40" s="49" t="s">
+      <c r="D40" s="48" t="s">
         <v>502</v>
       </c>
-      <c r="E40" s="40"/>
-      <c r="F40" s="41" t="s">
+      <c r="E40" s="39"/>
+      <c r="F40" s="40" t="s">
         <v>491</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="78"/>
-      <c r="B41" s="38" t="s">
+      <c r="A41" s="77"/>
+      <c r="B41" s="37" t="s">
         <v>488</v>
       </c>
-      <c r="C41" s="39" t="s">
+      <c r="C41" s="38" t="s">
         <v>476</v>
       </c>
-      <c r="D41" s="39" t="s">
+      <c r="D41" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="E41" s="40"/>
-      <c r="F41" s="41"/>
+      <c r="E41" s="39"/>
+      <c r="F41" s="40"/>
     </row>
     <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="78"/>
-      <c r="B42" s="38" t="s">
+      <c r="A42" s="77"/>
+      <c r="B42" s="37" t="s">
         <v>472</v>
       </c>
-      <c r="C42" s="39" t="s">
+      <c r="C42" s="38" t="s">
         <v>477</v>
       </c>
-      <c r="D42" s="39" t="s">
+      <c r="D42" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="E42" s="40"/>
-      <c r="F42" s="41" t="s">
+      <c r="E42" s="39"/>
+      <c r="F42" s="40" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="78"/>
-      <c r="B43" s="38" t="s">
+      <c r="A43" s="77"/>
+      <c r="B43" s="37" t="s">
         <v>529</v>
       </c>
-      <c r="C43" s="39" t="s">
+      <c r="C43" s="38" t="s">
         <v>531</v>
       </c>
-      <c r="D43" s="39" t="s">
+      <c r="D43" s="38" t="s">
         <v>530</v>
       </c>
-      <c r="E43" s="40"/>
-      <c r="F43" s="41" t="s">
+      <c r="E43" s="39"/>
+      <c r="F43" s="40" t="s">
         <v>501</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A44" s="78"/>
-      <c r="B44" s="38" t="s">
+      <c r="A44" s="77"/>
+      <c r="B44" s="37" t="s">
         <v>473</v>
       </c>
-      <c r="C44" s="38" t="s">
+      <c r="C44" s="37" t="s">
         <v>479</v>
       </c>
-      <c r="D44" s="39" t="s">
+      <c r="D44" s="38" t="s">
         <v>532</v>
       </c>
-      <c r="E44" s="40"/>
-      <c r="F44" s="41"/>
+      <c r="E44" s="39"/>
+      <c r="F44" s="40"/>
     </row>
     <row r="45" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A45" s="78"/>
-      <c r="B45" s="38" t="s">
+      <c r="A45" s="77"/>
+      <c r="B45" s="37" t="s">
         <v>474</v>
       </c>
-      <c r="C45" s="38" t="s">
+      <c r="C45" s="37" t="s">
         <v>480</v>
       </c>
-      <c r="D45" s="39" t="s">
+      <c r="D45" s="38" t="s">
         <v>481</v>
       </c>
-      <c r="E45" s="40"/>
-      <c r="F45" s="41"/>
+      <c r="E45" s="39"/>
+      <c r="F45" s="40"/>
     </row>
     <row r="46" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A46" s="78"/>
-      <c r="B46" s="46" t="s">
+      <c r="A46" s="77"/>
+      <c r="B46" s="45" t="s">
         <v>492</v>
       </c>
-      <c r="C46" s="46" t="s">
+      <c r="C46" s="45" t="s">
         <v>493</v>
       </c>
-      <c r="D46" s="47" t="s">
+      <c r="D46" s="46" t="s">
         <v>494</v>
       </c>
-      <c r="E46" s="50"/>
-      <c r="F46" s="51"/>
+      <c r="E46" s="49"/>
+      <c r="F46" s="50"/>
     </row>
     <row r="47" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A47" s="78"/>
-      <c r="B47" s="42" t="s">
+      <c r="A47" s="77"/>
+      <c r="B47" s="41" t="s">
         <v>475</v>
       </c>
-      <c r="C47" s="42" t="s">
+      <c r="C47" s="41" t="s">
         <v>482</v>
       </c>
-      <c r="D47" s="43" t="s">
+      <c r="D47" s="42" t="s">
         <v>483</v>
       </c>
-      <c r="E47" s="44"/>
-      <c r="F47" s="45"/>
+      <c r="E47" s="43"/>
+      <c r="F47" s="44"/>
     </row>
     <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="72" t="s">
+      <c r="A48" s="71" t="s">
         <v>105</v>
       </c>
-      <c r="B48" s="24" t="s">
+      <c r="B48" s="23" t="s">
         <v>503</v>
       </c>
-      <c r="C48" s="24" t="s">
+      <c r="C48" s="23" t="s">
         <v>504</v>
       </c>
-      <c r="D48" s="24" t="s">
+      <c r="D48" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="E48" s="25" t="s">
+      <c r="E48" s="24" t="s">
         <v>503</v>
       </c>
-      <c r="F48" s="26"/>
+      <c r="F48" s="25"/>
     </row>
     <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="72"/>
-      <c r="B49" s="24" t="s">
+      <c r="A49" s="71"/>
+      <c r="B49" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="C49" s="24" t="s">
+      <c r="C49" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="D49" s="24" t="s">
+      <c r="D49" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="E49" s="25" t="s">
+      <c r="E49" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="F49" s="52"/>
+      <c r="F49" s="51"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="72"/>
-      <c r="B50" s="27" t="s">
+      <c r="A50" s="71"/>
+      <c r="B50" s="26" t="s">
         <v>110</v>
       </c>
-      <c r="C50" s="27" t="s">
+      <c r="C50" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="D50" s="27" t="s">
+      <c r="D50" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="E50" s="28" t="s">
+      <c r="E50" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="F50" s="29"/>
+      <c r="F50" s="28"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="72"/>
-      <c r="B51" s="27" t="s">
+      <c r="A51" s="71"/>
+      <c r="B51" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="C51" s="27" t="s">
+      <c r="C51" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="D51" s="27" t="s">
+      <c r="D51" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="E51" s="28" t="s">
+      <c r="E51" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="F51" s="29"/>
+      <c r="F51" s="28"/>
     </row>
     <row r="52" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A52" s="72"/>
-      <c r="B52" s="27" t="s">
+      <c r="A52" s="71"/>
+      <c r="B52" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="C52" s="27" t="s">
+      <c r="C52" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="D52" s="29" t="s">
+      <c r="D52" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="E52" s="28" t="s">
+      <c r="E52" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="F52" s="29" t="s">
+      <c r="F52" s="28" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A53" s="72"/>
-      <c r="B53" s="27" t="s">
+      <c r="A53" s="71"/>
+      <c r="B53" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="C53" s="27" t="s">
+      <c r="C53" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="D53" s="29" t="s">
+      <c r="D53" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="E53" s="28" t="s">
+      <c r="E53" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="F53" s="29"/>
+      <c r="F53" s="28"/>
     </row>
     <row r="54" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A54" s="72"/>
-      <c r="B54" s="30" t="s">
+      <c r="A54" s="71"/>
+      <c r="B54" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="C54" s="30" t="s">
+      <c r="C54" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="D54" s="31" t="s">
+      <c r="D54" s="30" t="s">
         <v>534</v>
       </c>
-      <c r="E54" s="32" t="s">
+      <c r="E54" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="F54" s="31" t="s">
+      <c r="F54" s="30" t="s">
         <v>535</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A55" s="72"/>
+      <c r="A55" s="71"/>
       <c r="B55" s="15" t="s">
         <v>546</v>
       </c>
@@ -6133,13 +6155,13 @@
         <v>547</v>
       </c>
       <c r="D55" s="17"/>
-      <c r="E55" s="33"/>
+      <c r="E55" s="32"/>
       <c r="F55" s="17" t="s">
         <v>548</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="A56" s="72"/>
+      <c r="A56" s="71"/>
       <c r="B56" s="15" t="s">
         <v>460</v>
       </c>
@@ -6149,1699 +6171,1699 @@
       <c r="D56" s="17" t="s">
         <v>461</v>
       </c>
-      <c r="E56" s="33"/>
+      <c r="E56" s="32"/>
       <c r="F56" s="17" t="s">
         <v>533</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="73" t="s">
+      <c r="A57" s="72" t="s">
         <v>521</v>
       </c>
-      <c r="B57" s="53" t="s">
+      <c r="B57" s="52" t="s">
         <v>515</v>
       </c>
-      <c r="C57" s="53" t="s">
+      <c r="C57" s="52" t="s">
         <v>522</v>
       </c>
-      <c r="D57" s="54" t="s">
+      <c r="D57" s="53" t="s">
         <v>108</v>
       </c>
-      <c r="E57" s="55"/>
-      <c r="F57" s="54"/>
+      <c r="E57" s="54"/>
+      <c r="F57" s="53"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="73"/>
-      <c r="B58" s="53" t="s">
+      <c r="A58" s="72"/>
+      <c r="B58" s="52" t="s">
         <v>516</v>
       </c>
-      <c r="C58" s="53" t="s">
+      <c r="C58" s="52" t="s">
         <v>523</v>
       </c>
-      <c r="D58" s="54" t="s">
+      <c r="D58" s="53" t="s">
         <v>524</v>
       </c>
-      <c r="E58" s="55"/>
-      <c r="F58" s="54"/>
+      <c r="E58" s="54"/>
+      <c r="F58" s="53"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="73"/>
-      <c r="B59" s="53" t="s">
+      <c r="A59" s="72"/>
+      <c r="B59" s="52" t="s">
         <v>517</v>
       </c>
-      <c r="C59" s="53" t="s">
+      <c r="C59" s="52" t="s">
         <v>552</v>
       </c>
-      <c r="D59" s="54" t="s">
+      <c r="D59" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="E59" s="55"/>
-      <c r="F59" s="54"/>
+      <c r="E59" s="54"/>
+      <c r="F59" s="53"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="73"/>
-      <c r="B60" s="53" t="s">
+      <c r="A60" s="72"/>
+      <c r="B60" s="52" t="s">
         <v>518</v>
       </c>
-      <c r="C60" s="53" t="s">
+      <c r="C60" s="52" t="s">
         <v>553</v>
       </c>
-      <c r="D60" s="54" t="s">
+      <c r="D60" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="E60" s="55"/>
-      <c r="F60" s="54"/>
+      <c r="E60" s="54"/>
+      <c r="F60" s="53"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="73"/>
-      <c r="B61" s="53" t="s">
+      <c r="A61" s="72"/>
+      <c r="B61" s="52" t="s">
         <v>519</v>
       </c>
-      <c r="C61" s="53" t="s">
+      <c r="C61" s="52" t="s">
         <v>525</v>
       </c>
-      <c r="D61" s="54"/>
-      <c r="E61" s="55"/>
-      <c r="F61" s="54"/>
+      <c r="D61" s="53"/>
+      <c r="E61" s="54"/>
+      <c r="F61" s="53"/>
     </row>
     <row r="62" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A62" s="73"/>
-      <c r="B62" s="53" t="s">
+      <c r="A62" s="72"/>
+      <c r="B62" s="52" t="s">
         <v>520</v>
       </c>
-      <c r="C62" s="53" t="s">
+      <c r="C62" s="52" t="s">
         <v>526</v>
       </c>
-      <c r="D62" s="54" t="s">
+      <c r="D62" s="53" t="s">
         <v>528</v>
       </c>
-      <c r="E62" s="55"/>
-      <c r="F62" s="54" t="s">
+      <c r="E62" s="54"/>
+      <c r="F62" s="53" t="s">
         <v>527</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="72" t="s">
+      <c r="A63" s="71" t="s">
         <v>127</v>
       </c>
-      <c r="B63" s="56" t="s">
+      <c r="B63" s="55" t="s">
         <v>128</v>
       </c>
-      <c r="C63" s="56" t="s">
+      <c r="C63" s="55" t="s">
         <v>129</v>
       </c>
-      <c r="D63" s="56" t="s">
+      <c r="D63" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="E63" s="57" t="s">
+      <c r="E63" s="56" t="s">
         <v>130</v>
       </c>
-      <c r="F63" s="58"/>
+      <c r="F63" s="57"/>
     </row>
     <row r="64" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A64" s="72"/>
-      <c r="B64" s="59" t="s">
+      <c r="A64" s="71"/>
+      <c r="B64" s="58" t="s">
         <v>131</v>
       </c>
-      <c r="C64" s="59" t="s">
+      <c r="C64" s="58" t="s">
         <v>132</v>
       </c>
-      <c r="D64" s="60" t="s">
+      <c r="D64" s="59" t="s">
         <v>333</v>
       </c>
-      <c r="E64" s="61" t="s">
+      <c r="E64" s="60" t="s">
         <v>131</v>
       </c>
-      <c r="F64" s="60" t="s">
+      <c r="F64" s="59" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A65" s="72"/>
-      <c r="B65" s="59" t="s">
+      <c r="A65" s="71"/>
+      <c r="B65" s="58" t="s">
         <v>505</v>
       </c>
-      <c r="C65" s="60" t="s">
+      <c r="C65" s="59" t="s">
         <v>513</v>
       </c>
-      <c r="D65" s="60" t="s">
+      <c r="D65" s="59" t="s">
         <v>108</v>
       </c>
-      <c r="E65" s="61"/>
-      <c r="F65" s="60" t="s">
+      <c r="E65" s="60"/>
+      <c r="F65" s="59" t="s">
         <v>507</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A66" s="72"/>
-      <c r="B66" s="59" t="s">
+      <c r="A66" s="71"/>
+      <c r="B66" s="58" t="s">
         <v>506</v>
       </c>
-      <c r="C66" s="60" t="s">
+      <c r="C66" s="59" t="s">
         <v>514</v>
       </c>
-      <c r="D66" s="60" t="s">
+      <c r="D66" s="59" t="s">
         <v>108</v>
       </c>
-      <c r="E66" s="61"/>
-      <c r="F66" s="60" t="s">
+      <c r="E66" s="60"/>
+      <c r="F66" s="59" t="s">
         <v>508</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A67" s="72"/>
-      <c r="B67" s="59" t="s">
+      <c r="A67" s="71"/>
+      <c r="B67" s="58" t="s">
         <v>134</v>
       </c>
-      <c r="C67" s="60" t="s">
+      <c r="C67" s="59" t="s">
         <v>335</v>
       </c>
-      <c r="D67" s="60" t="s">
+      <c r="D67" s="59" t="s">
         <v>336</v>
       </c>
-      <c r="E67" s="61" t="s">
+      <c r="E67" s="60" t="s">
         <v>134</v>
       </c>
-      <c r="F67" s="60"/>
+      <c r="F67" s="59"/>
     </row>
     <row r="68" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A68" s="72"/>
-      <c r="B68" s="59" t="s">
+      <c r="A68" s="71"/>
+      <c r="B68" s="58" t="s">
         <v>137</v>
       </c>
-      <c r="C68" s="60" t="s">
+      <c r="C68" s="59" t="s">
         <v>337</v>
       </c>
-      <c r="D68" s="59" t="s">
+      <c r="D68" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E68" s="61" t="s">
+      <c r="E68" s="60" t="s">
         <v>137</v>
       </c>
-      <c r="F68" s="60"/>
+      <c r="F68" s="59"/>
     </row>
     <row r="69" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A69" s="72"/>
-      <c r="B69" s="59" t="s">
+      <c r="A69" s="71"/>
+      <c r="B69" s="58" t="s">
         <v>139</v>
       </c>
-      <c r="C69" s="60" t="s">
+      <c r="C69" s="59" t="s">
         <v>338</v>
       </c>
-      <c r="D69" s="59" t="s">
+      <c r="D69" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E69" s="61" t="s">
+      <c r="E69" s="60" t="s">
         <v>139</v>
       </c>
-      <c r="F69" s="60"/>
+      <c r="F69" s="59"/>
     </row>
     <row r="70" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A70" s="72"/>
-      <c r="B70" s="59" t="s">
+      <c r="A70" s="71"/>
+      <c r="B70" s="58" t="s">
         <v>141</v>
       </c>
-      <c r="C70" s="60" t="s">
+      <c r="C70" s="59" t="s">
         <v>339</v>
       </c>
-      <c r="D70" s="60" t="s">
+      <c r="D70" s="59" t="s">
         <v>340</v>
       </c>
-      <c r="E70" s="61" t="s">
+      <c r="E70" s="60" t="s">
         <v>141</v>
       </c>
-      <c r="F70" s="60"/>
+      <c r="F70" s="59"/>
     </row>
     <row r="71" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A71" s="72"/>
-      <c r="B71" s="59" t="s">
+      <c r="A71" s="71"/>
+      <c r="B71" s="58" t="s">
         <v>144</v>
       </c>
-      <c r="C71" s="60" t="s">
+      <c r="C71" s="59" t="s">
         <v>341</v>
       </c>
-      <c r="D71" s="60" t="s">
+      <c r="D71" s="59" t="s">
         <v>342</v>
       </c>
-      <c r="E71" s="61" t="s">
+      <c r="E71" s="60" t="s">
         <v>144</v>
       </c>
-      <c r="F71" s="60" t="s">
+      <c r="F71" s="59" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A72" s="72"/>
-      <c r="B72" s="59" t="s">
+      <c r="A72" s="71"/>
+      <c r="B72" s="58" t="s">
         <v>148</v>
       </c>
-      <c r="C72" s="60" t="s">
+      <c r="C72" s="59" t="s">
         <v>343</v>
       </c>
-      <c r="D72" s="59" t="s">
+      <c r="D72" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="E72" s="61" t="s">
+      <c r="E72" s="60" t="s">
         <v>148</v>
       </c>
-      <c r="F72" s="60"/>
+      <c r="F72" s="59"/>
     </row>
     <row r="73" spans="1:6" ht="150" x14ac:dyDescent="0.25">
-      <c r="A73" s="72"/>
-      <c r="B73" s="59" t="s">
+      <c r="A73" s="71"/>
+      <c r="B73" s="58" t="s">
         <v>443</v>
       </c>
-      <c r="C73" s="60" t="s">
+      <c r="C73" s="59" t="s">
         <v>445</v>
       </c>
-      <c r="D73" s="59" t="s">
+      <c r="D73" s="58" t="s">
         <v>536</v>
       </c>
-      <c r="E73" s="61"/>
-      <c r="F73" s="60" t="s">
+      <c r="E73" s="60"/>
+      <c r="F73" s="59" t="s">
         <v>462</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="A74" s="72"/>
-      <c r="B74" s="59" t="s">
+      <c r="A74" s="71"/>
+      <c r="B74" s="58" t="s">
         <v>150</v>
       </c>
-      <c r="C74" s="60" t="s">
+      <c r="C74" s="59" t="s">
         <v>344</v>
       </c>
-      <c r="D74" s="60" t="s">
+      <c r="D74" s="59" t="s">
         <v>345</v>
       </c>
-      <c r="E74" s="61" t="s">
+      <c r="E74" s="60" t="s">
         <v>153</v>
       </c>
-      <c r="F74" s="60"/>
+      <c r="F74" s="59"/>
     </row>
     <row r="75" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A75" s="72"/>
-      <c r="B75" s="59" t="s">
+      <c r="A75" s="71"/>
+      <c r="B75" s="58" t="s">
         <v>154</v>
       </c>
-      <c r="C75" s="60" t="s">
+      <c r="C75" s="59" t="s">
         <v>346</v>
       </c>
-      <c r="D75" s="60" t="s">
+      <c r="D75" s="59" t="s">
         <v>347</v>
       </c>
-      <c r="E75" s="61" t="s">
+      <c r="E75" s="60" t="s">
         <v>157</v>
       </c>
-      <c r="F75" s="60"/>
+      <c r="F75" s="59"/>
     </row>
     <row r="76" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A76" s="72"/>
-      <c r="B76" s="59" t="s">
+      <c r="A76" s="71"/>
+      <c r="B76" s="58" t="s">
         <v>158</v>
       </c>
-      <c r="C76" s="60" t="s">
+      <c r="C76" s="59" t="s">
         <v>348</v>
       </c>
-      <c r="D76" s="59" t="s">
+      <c r="D76" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="E76" s="61" t="s">
+      <c r="E76" s="60" t="s">
         <v>158</v>
       </c>
-      <c r="F76" s="60"/>
+      <c r="F76" s="59"/>
     </row>
     <row r="77" spans="1:6" ht="165" x14ac:dyDescent="0.25">
-      <c r="A77" s="72"/>
-      <c r="B77" s="59" t="s">
+      <c r="A77" s="71"/>
+      <c r="B77" s="58" t="s">
         <v>442</v>
       </c>
-      <c r="C77" s="60" t="s">
+      <c r="C77" s="59" t="s">
         <v>444</v>
       </c>
-      <c r="D77" s="59" t="s">
+      <c r="D77" s="58" t="s">
         <v>550</v>
       </c>
-      <c r="E77" s="61"/>
-      <c r="F77" s="60" t="s">
+      <c r="E77" s="60"/>
+      <c r="F77" s="59" t="s">
         <v>549</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A78" s="72"/>
-      <c r="B78" s="59" t="s">
+      <c r="A78" s="71"/>
+      <c r="B78" s="58" t="s">
         <v>495</v>
       </c>
-      <c r="C78" s="60" t="s">
+      <c r="C78" s="59" t="s">
         <v>496</v>
       </c>
-      <c r="D78" s="60" t="s">
+      <c r="D78" s="59" t="s">
         <v>551</v>
       </c>
-      <c r="E78" s="61"/>
-      <c r="F78" s="60" t="s">
+      <c r="E78" s="60"/>
+      <c r="F78" s="59" t="s">
         <v>497</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="180" x14ac:dyDescent="0.25">
-      <c r="A79" s="72"/>
-      <c r="B79" s="59" t="s">
+      <c r="A79" s="71"/>
+      <c r="B79" s="58" t="s">
         <v>160</v>
       </c>
-      <c r="C79" s="60" t="s">
+      <c r="C79" s="59" t="s">
         <v>349</v>
       </c>
-      <c r="D79" s="60" t="s">
+      <c r="D79" s="59" t="s">
         <v>350</v>
       </c>
-      <c r="E79" s="61" t="s">
+      <c r="E79" s="60" t="s">
         <v>160</v>
       </c>
-      <c r="F79" s="60"/>
+      <c r="F79" s="59"/>
     </row>
     <row r="80" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A80" s="72"/>
-      <c r="B80" s="59" t="s">
+      <c r="A80" s="71"/>
+      <c r="B80" s="58" t="s">
         <v>163</v>
       </c>
-      <c r="C80" s="60" t="s">
+      <c r="C80" s="59" t="s">
         <v>351</v>
       </c>
-      <c r="D80" s="59" t="s">
+      <c r="D80" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E80" s="61" t="s">
+      <c r="E80" s="60" t="s">
         <v>165</v>
       </c>
-      <c r="F80" s="60"/>
+      <c r="F80" s="59"/>
     </row>
     <row r="81" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A81" s="72"/>
-      <c r="B81" s="59" t="s">
+      <c r="A81" s="71"/>
+      <c r="B81" s="58" t="s">
         <v>166</v>
       </c>
-      <c r="C81" s="60" t="s">
+      <c r="C81" s="59" t="s">
         <v>352</v>
       </c>
-      <c r="D81" s="60" t="s">
+      <c r="D81" s="59" t="s">
         <v>353</v>
       </c>
-      <c r="E81" s="61" t="s">
+      <c r="E81" s="60" t="s">
         <v>166</v>
       </c>
-      <c r="F81" s="60"/>
+      <c r="F81" s="59"/>
     </row>
     <row r="82" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A82" s="72"/>
-      <c r="B82" s="59" t="s">
+      <c r="A82" s="71"/>
+      <c r="B82" s="58" t="s">
         <v>169</v>
       </c>
-      <c r="C82" s="60" t="s">
+      <c r="C82" s="59" t="s">
         <v>354</v>
       </c>
-      <c r="D82" s="59" t="s">
+      <c r="D82" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E82" s="61" t="s">
+      <c r="E82" s="60" t="s">
         <v>169</v>
       </c>
-      <c r="F82" s="60"/>
+      <c r="F82" s="59"/>
     </row>
     <row r="83" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="A83" s="72"/>
-      <c r="B83" s="59" t="s">
+      <c r="A83" s="71"/>
+      <c r="B83" s="58" t="s">
         <v>171</v>
       </c>
-      <c r="C83" s="60" t="s">
+      <c r="C83" s="59" t="s">
         <v>355</v>
       </c>
-      <c r="D83" s="59" t="s">
+      <c r="D83" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E83" s="61"/>
-      <c r="F83" s="60" t="s">
+      <c r="E83" s="60"/>
+      <c r="F83" s="59" t="s">
         <v>356</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="72"/>
-      <c r="B84" s="59" t="s">
+      <c r="A84" s="71"/>
+      <c r="B84" s="58" t="s">
         <v>173</v>
       </c>
-      <c r="C84" s="60" t="s">
+      <c r="C84" s="59" t="s">
         <v>357</v>
       </c>
-      <c r="D84" s="59" t="s">
+      <c r="D84" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E84" s="61"/>
-      <c r="F84" s="60"/>
+      <c r="E84" s="60"/>
+      <c r="F84" s="59"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="72"/>
-      <c r="B85" s="59" t="s">
+      <c r="A85" s="71"/>
+      <c r="B85" s="58" t="s">
         <v>175</v>
       </c>
-      <c r="C85" s="59" t="s">
+      <c r="C85" s="58" t="s">
         <v>176</v>
       </c>
-      <c r="D85" s="59" t="s">
+      <c r="D85" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="E85" s="61" t="s">
+      <c r="E85" s="60" t="s">
         <v>175</v>
       </c>
-      <c r="F85" s="60"/>
+      <c r="F85" s="59"/>
     </row>
     <row r="86" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A86" s="72"/>
-      <c r="B86" s="59" t="s">
+      <c r="A86" s="71"/>
+      <c r="B86" s="58" t="s">
         <v>178</v>
       </c>
-      <c r="C86" s="60" t="s">
+      <c r="C86" s="59" t="s">
         <v>358</v>
       </c>
-      <c r="D86" s="59" t="s">
+      <c r="D86" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="E86" s="61" t="s">
+      <c r="E86" s="60" t="s">
         <v>178</v>
       </c>
-      <c r="F86" s="60"/>
+      <c r="F86" s="59"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="72"/>
-      <c r="B87" s="59" t="s">
+      <c r="A87" s="71"/>
+      <c r="B87" s="58" t="s">
         <v>180</v>
       </c>
-      <c r="C87" s="59" t="s">
+      <c r="C87" s="58" t="s">
         <v>181</v>
       </c>
-      <c r="D87" s="59" t="s">
+      <c r="D87" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="E87" s="61" t="s">
+      <c r="E87" s="60" t="s">
         <v>180</v>
       </c>
-      <c r="F87" s="60"/>
+      <c r="F87" s="59"/>
     </row>
     <row r="88" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A88" s="72"/>
-      <c r="B88" s="59" t="s">
+      <c r="A88" s="71"/>
+      <c r="B88" s="58" t="s">
         <v>182</v>
       </c>
-      <c r="C88" s="60" t="s">
+      <c r="C88" s="59" t="s">
         <v>359</v>
       </c>
-      <c r="D88" s="59" t="s">
+      <c r="D88" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="E88" s="61" t="s">
+      <c r="E88" s="60" t="s">
         <v>182</v>
       </c>
-      <c r="F88" s="60"/>
+      <c r="F88" s="59"/>
     </row>
     <row r="89" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A89" s="72"/>
-      <c r="B89" s="59" t="s">
+      <c r="A89" s="71"/>
+      <c r="B89" s="58" t="s">
         <v>184</v>
       </c>
-      <c r="C89" s="60" t="s">
+      <c r="C89" s="59" t="s">
         <v>360</v>
       </c>
-      <c r="D89" s="59" t="s">
+      <c r="D89" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E89" s="61" t="s">
+      <c r="E89" s="60" t="s">
         <v>184</v>
       </c>
-      <c r="F89" s="60"/>
+      <c r="F89" s="59"/>
     </row>
     <row r="90" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A90" s="72"/>
-      <c r="B90" s="59" t="s">
+      <c r="A90" s="71"/>
+      <c r="B90" s="58" t="s">
         <v>186</v>
       </c>
-      <c r="C90" s="60" t="s">
+      <c r="C90" s="59" t="s">
         <v>361</v>
       </c>
-      <c r="D90" s="59" t="s">
+      <c r="D90" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E90" s="61" t="s">
+      <c r="E90" s="60" t="s">
         <v>186</v>
       </c>
-      <c r="F90" s="60"/>
+      <c r="F90" s="59"/>
     </row>
     <row r="91" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A91" s="72"/>
-      <c r="B91" s="59" t="s">
+      <c r="A91" s="71"/>
+      <c r="B91" s="58" t="s">
         <v>188</v>
       </c>
-      <c r="C91" s="60" t="s">
+      <c r="C91" s="59" t="s">
         <v>362</v>
       </c>
-      <c r="D91" s="60" t="s">
+      <c r="D91" s="59" t="s">
         <v>340</v>
       </c>
-      <c r="E91" s="61" t="s">
+      <c r="E91" s="60" t="s">
         <v>188</v>
       </c>
-      <c r="F91" s="60"/>
+      <c r="F91" s="59"/>
     </row>
     <row r="92" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A92" s="72"/>
-      <c r="B92" s="59" t="s">
+      <c r="A92" s="71"/>
+      <c r="B92" s="58" t="s">
         <v>190</v>
       </c>
-      <c r="C92" s="60" t="s">
+      <c r="C92" s="59" t="s">
         <v>363</v>
       </c>
-      <c r="D92" s="60" t="s">
+      <c r="D92" s="59" t="s">
         <v>342</v>
       </c>
-      <c r="E92" s="61"/>
-      <c r="F92" s="60"/>
+      <c r="E92" s="60"/>
+      <c r="F92" s="59"/>
     </row>
     <row r="93" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A93" s="72"/>
-      <c r="B93" s="59" t="s">
+      <c r="A93" s="71"/>
+      <c r="B93" s="58" t="s">
         <v>193</v>
       </c>
-      <c r="C93" s="60" t="s">
+      <c r="C93" s="59" t="s">
         <v>364</v>
       </c>
-      <c r="D93" s="59" t="s">
+      <c r="D93" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="E93" s="61" t="s">
+      <c r="E93" s="60" t="s">
         <v>193</v>
       </c>
-      <c r="F93" s="60"/>
+      <c r="F93" s="59"/>
     </row>
     <row r="94" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="72"/>
-      <c r="B94" s="59" t="s">
+      <c r="A94" s="71"/>
+      <c r="B94" s="58" t="s">
         <v>447</v>
       </c>
-      <c r="C94" s="60" t="s">
+      <c r="C94" s="59" t="s">
         <v>448</v>
       </c>
-      <c r="D94" s="59" t="s">
+      <c r="D94" s="58" t="s">
         <v>446</v>
       </c>
-      <c r="E94" s="61"/>
-      <c r="F94" s="59" t="s">
+      <c r="E94" s="60"/>
+      <c r="F94" s="58" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="A95" s="72"/>
-      <c r="B95" s="59" t="s">
+      <c r="A95" s="71"/>
+      <c r="B95" s="58" t="s">
         <v>195</v>
       </c>
-      <c r="C95" s="60" t="s">
+      <c r="C95" s="59" t="s">
         <v>365</v>
       </c>
-      <c r="D95" s="60" t="s">
+      <c r="D95" s="59" t="s">
         <v>345</v>
       </c>
-      <c r="E95" s="61" t="s">
+      <c r="E95" s="60" t="s">
         <v>197</v>
       </c>
-      <c r="F95" s="60"/>
+      <c r="F95" s="59"/>
     </row>
     <row r="96" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A96" s="72"/>
-      <c r="B96" s="59" t="s">
+      <c r="A96" s="71"/>
+      <c r="B96" s="58" t="s">
         <v>198</v>
       </c>
-      <c r="C96" s="60" t="s">
+      <c r="C96" s="59" t="s">
         <v>366</v>
       </c>
-      <c r="D96" s="60" t="s">
+      <c r="D96" s="59" t="s">
         <v>347</v>
       </c>
-      <c r="E96" s="61" t="s">
+      <c r="E96" s="60" t="s">
         <v>200</v>
       </c>
-      <c r="F96" s="60"/>
+      <c r="F96" s="59"/>
     </row>
     <row r="97" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A97" s="72"/>
-      <c r="B97" s="59" t="s">
+      <c r="A97" s="71"/>
+      <c r="B97" s="58" t="s">
         <v>201</v>
       </c>
-      <c r="C97" s="60" t="s">
+      <c r="C97" s="59" t="s">
         <v>367</v>
       </c>
-      <c r="D97" s="59" t="s">
+      <c r="D97" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="E97" s="61"/>
-      <c r="F97" s="60"/>
+      <c r="E97" s="60"/>
+      <c r="F97" s="59"/>
     </row>
     <row r="98" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="72"/>
-      <c r="B98" s="59" t="s">
+      <c r="A98" s="71"/>
+      <c r="B98" s="58" t="s">
         <v>451</v>
       </c>
-      <c r="C98" s="60" t="s">
+      <c r="C98" s="59" t="s">
         <v>452</v>
       </c>
-      <c r="D98" s="59" t="s">
+      <c r="D98" s="58" t="s">
         <v>550</v>
       </c>
-      <c r="E98" s="61"/>
-      <c r="F98" s="60" t="s">
+      <c r="E98" s="60"/>
+      <c r="F98" s="59" t="s">
         <v>464</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A99" s="72"/>
-      <c r="B99" s="59" t="s">
+      <c r="A99" s="71"/>
+      <c r="B99" s="58" t="s">
         <v>498</v>
       </c>
-      <c r="C99" s="60" t="s">
+      <c r="C99" s="59" t="s">
         <v>496</v>
       </c>
-      <c r="D99" s="60" t="s">
+      <c r="D99" s="59" t="s">
         <v>551</v>
       </c>
-      <c r="E99" s="61"/>
-      <c r="F99" s="60" t="s">
+      <c r="E99" s="60"/>
+      <c r="F99" s="59" t="s">
         <v>497</v>
       </c>
     </row>
     <row r="100" spans="1:6" ht="180" x14ac:dyDescent="0.25">
-      <c r="A100" s="72"/>
-      <c r="B100" s="59" t="s">
+      <c r="A100" s="71"/>
+      <c r="B100" s="58" t="s">
         <v>203</v>
       </c>
-      <c r="C100" s="60" t="s">
+      <c r="C100" s="59" t="s">
         <v>368</v>
       </c>
-      <c r="D100" s="60" t="s">
+      <c r="D100" s="59" t="s">
         <v>350</v>
       </c>
-      <c r="E100" s="61" t="s">
+      <c r="E100" s="60" t="s">
         <v>203</v>
       </c>
-      <c r="F100" s="60"/>
+      <c r="F100" s="59"/>
     </row>
     <row r="101" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A101" s="72"/>
-      <c r="B101" s="59" t="s">
+      <c r="A101" s="71"/>
+      <c r="B101" s="58" t="s">
         <v>205</v>
       </c>
-      <c r="C101" s="60" t="s">
+      <c r="C101" s="59" t="s">
         <v>369</v>
       </c>
-      <c r="D101" s="59" t="s">
+      <c r="D101" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E101" s="61" t="s">
+      <c r="E101" s="60" t="s">
         <v>207</v>
       </c>
-      <c r="F101" s="60"/>
+      <c r="F101" s="59"/>
     </row>
     <row r="102" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A102" s="72"/>
-      <c r="B102" s="59" t="s">
+      <c r="A102" s="71"/>
+      <c r="B102" s="58" t="s">
         <v>208</v>
       </c>
-      <c r="C102" s="60" t="s">
+      <c r="C102" s="59" t="s">
         <v>370</v>
       </c>
-      <c r="D102" s="60" t="s">
+      <c r="D102" s="59" t="s">
         <v>353</v>
       </c>
-      <c r="E102" s="61" t="s">
+      <c r="E102" s="60" t="s">
         <v>208</v>
       </c>
-      <c r="F102" s="60"/>
+      <c r="F102" s="59"/>
     </row>
     <row r="103" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A103" s="72"/>
-      <c r="B103" s="59" t="s">
+      <c r="A103" s="71"/>
+      <c r="B103" s="58" t="s">
         <v>210</v>
       </c>
-      <c r="C103" s="60" t="s">
+      <c r="C103" s="59" t="s">
         <v>371</v>
       </c>
-      <c r="D103" s="59" t="s">
+      <c r="D103" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E103" s="61"/>
-      <c r="F103" s="60"/>
+      <c r="E103" s="60"/>
+      <c r="F103" s="59"/>
     </row>
     <row r="104" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A104" s="72"/>
-      <c r="B104" s="59" t="s">
+      <c r="A104" s="71"/>
+      <c r="B104" s="58" t="s">
         <v>212</v>
       </c>
-      <c r="C104" s="60" t="s">
+      <c r="C104" s="59" t="s">
         <v>372</v>
       </c>
-      <c r="D104" s="59" t="s">
+      <c r="D104" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E104" s="61"/>
-      <c r="F104" s="60" t="s">
+      <c r="E104" s="60"/>
+      <c r="F104" s="59" t="s">
         <v>373</v>
       </c>
     </row>
     <row r="105" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A105" s="72"/>
-      <c r="B105" s="59" t="s">
+      <c r="A105" s="71"/>
+      <c r="B105" s="58" t="s">
         <v>214</v>
       </c>
-      <c r="C105" s="60" t="s">
+      <c r="C105" s="59" t="s">
         <v>374</v>
       </c>
-      <c r="D105" s="59" t="s">
+      <c r="D105" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E105" s="61"/>
-      <c r="F105" s="60"/>
+      <c r="E105" s="60"/>
+      <c r="F105" s="59"/>
     </row>
     <row r="106" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A106" s="72"/>
-      <c r="B106" s="59" t="s">
+      <c r="A106" s="71"/>
+      <c r="B106" s="58" t="s">
         <v>216</v>
       </c>
-      <c r="C106" s="60" t="s">
+      <c r="C106" s="59" t="s">
         <v>375</v>
       </c>
-      <c r="D106" s="59" t="s">
+      <c r="D106" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E106" s="61"/>
-      <c r="F106" s="60"/>
+      <c r="E106" s="60"/>
+      <c r="F106" s="59"/>
     </row>
     <row r="107" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A107" s="72"/>
-      <c r="B107" s="59" t="s">
+      <c r="A107" s="71"/>
+      <c r="B107" s="58" t="s">
         <v>218</v>
       </c>
-      <c r="C107" s="60" t="s">
+      <c r="C107" s="59" t="s">
         <v>376</v>
       </c>
-      <c r="D107" s="59" t="s">
+      <c r="D107" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E107" s="61"/>
-      <c r="F107" s="60"/>
+      <c r="E107" s="60"/>
+      <c r="F107" s="59"/>
     </row>
     <row r="108" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A108" s="72"/>
-      <c r="B108" s="59" t="s">
+      <c r="A108" s="71"/>
+      <c r="B108" s="58" t="s">
         <v>220</v>
       </c>
-      <c r="C108" s="59" t="s">
+      <c r="C108" s="58" t="s">
         <v>221</v>
       </c>
-      <c r="D108" s="59" t="s">
+      <c r="D108" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E108" s="61"/>
-      <c r="F108" s="60" t="s">
+      <c r="E108" s="60"/>
+      <c r="F108" s="59" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" s="72"/>
-      <c r="B109" s="59" t="s">
+      <c r="A109" s="71"/>
+      <c r="B109" s="58" t="s">
         <v>222</v>
       </c>
-      <c r="C109" s="59" t="s">
+      <c r="C109" s="58" t="s">
         <v>223</v>
       </c>
-      <c r="D109" s="59" t="s">
+      <c r="D109" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E109" s="61"/>
-      <c r="F109" s="60"/>
+      <c r="E109" s="60"/>
+      <c r="F109" s="59"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A110" s="72"/>
-      <c r="B110" s="59" t="s">
+      <c r="A110" s="71"/>
+      <c r="B110" s="58" t="s">
         <v>459</v>
       </c>
-      <c r="C110" s="59" t="s">
+      <c r="C110" s="58" t="s">
         <v>465</v>
       </c>
-      <c r="D110" s="59" t="s">
+      <c r="D110" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E110" s="61"/>
-      <c r="F110" s="60"/>
+      <c r="E110" s="60"/>
+      <c r="F110" s="59"/>
     </row>
     <row r="111" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A111" s="72"/>
-      <c r="B111" s="59" t="s">
+      <c r="A111" s="71"/>
+      <c r="B111" s="58" t="s">
         <v>470</v>
       </c>
-      <c r="C111" s="60" t="s">
+      <c r="C111" s="59" t="s">
         <v>422</v>
       </c>
-      <c r="D111" s="59" t="s">
+      <c r="D111" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E111" s="61"/>
-      <c r="F111" s="60"/>
+      <c r="E111" s="60"/>
+      <c r="F111" s="59"/>
     </row>
     <row r="112" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A112" s="72"/>
-      <c r="B112" s="59" t="s">
+      <c r="A112" s="71"/>
+      <c r="B112" s="58" t="s">
         <v>228</v>
       </c>
-      <c r="C112" s="60" t="s">
+      <c r="C112" s="59" t="s">
         <v>423</v>
       </c>
-      <c r="D112" s="59" t="s">
+      <c r="D112" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E112" s="61"/>
-      <c r="F112" s="60"/>
+      <c r="E112" s="60"/>
+      <c r="F112" s="59"/>
     </row>
     <row r="113" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A113" s="72"/>
-      <c r="B113" s="59" t="s">
+      <c r="A113" s="71"/>
+      <c r="B113" s="58" t="s">
         <v>230</v>
       </c>
-      <c r="C113" s="60" t="s">
+      <c r="C113" s="59" t="s">
         <v>424</v>
       </c>
-      <c r="D113" s="59" t="s">
+      <c r="D113" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E113" s="61"/>
-      <c r="F113" s="60"/>
+      <c r="E113" s="60"/>
+      <c r="F113" s="59"/>
     </row>
     <row r="114" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A114" s="72"/>
-      <c r="B114" s="59" t="s">
+      <c r="A114" s="71"/>
+      <c r="B114" s="58" t="s">
         <v>232</v>
       </c>
-      <c r="C114" s="59" t="s">
+      <c r="C114" s="58" t="s">
         <v>233</v>
       </c>
-      <c r="D114" s="60" t="s">
+      <c r="D114" s="59" t="s">
         <v>378</v>
       </c>
-      <c r="E114" s="61" t="s">
+      <c r="E114" s="60" t="s">
         <v>232</v>
       </c>
-      <c r="F114" s="60" t="s">
+      <c r="F114" s="59" t="s">
         <v>379</v>
       </c>
     </row>
     <row r="115" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A115" s="72"/>
-      <c r="B115" s="59" t="s">
+      <c r="A115" s="71"/>
+      <c r="B115" s="58" t="s">
         <v>509</v>
       </c>
-      <c r="C115" s="60" t="s">
+      <c r="C115" s="59" t="s">
         <v>511</v>
       </c>
-      <c r="D115" s="60" t="s">
+      <c r="D115" s="59" t="s">
         <v>108</v>
       </c>
-      <c r="E115" s="61"/>
-      <c r="F115" s="60" t="s">
+      <c r="E115" s="60"/>
+      <c r="F115" s="59" t="s">
         <v>507</v>
       </c>
     </row>
     <row r="116" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A116" s="72"/>
-      <c r="B116" s="59" t="s">
+      <c r="A116" s="71"/>
+      <c r="B116" s="58" t="s">
         <v>510</v>
       </c>
-      <c r="C116" s="60" t="s">
+      <c r="C116" s="59" t="s">
         <v>512</v>
       </c>
-      <c r="D116" s="60" t="s">
+      <c r="D116" s="59" t="s">
         <v>108</v>
       </c>
-      <c r="E116" s="61"/>
-      <c r="F116" s="60" t="s">
+      <c r="E116" s="60"/>
+      <c r="F116" s="59" t="s">
         <v>508</v>
       </c>
     </row>
     <row r="117" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A117" s="72"/>
-      <c r="B117" s="59" t="s">
+      <c r="A117" s="71"/>
+      <c r="B117" s="58" t="s">
         <v>234</v>
       </c>
-      <c r="C117" s="60" t="s">
+      <c r="C117" s="59" t="s">
         <v>380</v>
       </c>
-      <c r="D117" s="60" t="s">
+      <c r="D117" s="59" t="s">
         <v>336</v>
       </c>
-      <c r="E117" s="61"/>
-      <c r="F117" s="60"/>
+      <c r="E117" s="60"/>
+      <c r="F117" s="59"/>
     </row>
     <row r="118" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A118" s="72"/>
-      <c r="B118" s="59" t="s">
+      <c r="A118" s="71"/>
+      <c r="B118" s="58" t="s">
         <v>236</v>
       </c>
-      <c r="C118" s="60" t="s">
+      <c r="C118" s="59" t="s">
         <v>381</v>
       </c>
-      <c r="D118" s="59" t="s">
+      <c r="D118" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E118" s="61"/>
-      <c r="F118" s="60"/>
+      <c r="E118" s="60"/>
+      <c r="F118" s="59"/>
     </row>
     <row r="119" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A119" s="72"/>
-      <c r="B119" s="59" t="s">
+      <c r="A119" s="71"/>
+      <c r="B119" s="58" t="s">
         <v>238</v>
       </c>
-      <c r="C119" s="60" t="s">
+      <c r="C119" s="59" t="s">
         <v>382</v>
       </c>
-      <c r="D119" s="59" t="s">
+      <c r="D119" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E119" s="61"/>
-      <c r="F119" s="60"/>
+      <c r="E119" s="60"/>
+      <c r="F119" s="59"/>
     </row>
     <row r="120" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A120" s="72"/>
-      <c r="B120" s="59" t="s">
+      <c r="A120" s="71"/>
+      <c r="B120" s="58" t="s">
         <v>240</v>
       </c>
-      <c r="C120" s="60" t="s">
+      <c r="C120" s="59" t="s">
         <v>383</v>
       </c>
-      <c r="D120" s="60" t="s">
+      <c r="D120" s="59" t="s">
         <v>340</v>
       </c>
-      <c r="E120" s="61" t="s">
+      <c r="E120" s="60" t="s">
         <v>240</v>
       </c>
-      <c r="F120" s="60"/>
+      <c r="F120" s="59"/>
     </row>
     <row r="121" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A121" s="72"/>
-      <c r="B121" s="59" t="s">
+      <c r="A121" s="71"/>
+      <c r="B121" s="58" t="s">
         <v>242</v>
       </c>
-      <c r="C121" s="60" t="s">
+      <c r="C121" s="59" t="s">
         <v>384</v>
       </c>
-      <c r="D121" s="60" t="s">
+      <c r="D121" s="59" t="s">
         <v>342</v>
       </c>
-      <c r="E121" s="61"/>
-      <c r="F121" s="60"/>
+      <c r="E121" s="60"/>
+      <c r="F121" s="59"/>
     </row>
     <row r="122" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A122" s="72"/>
-      <c r="B122" s="59" t="s">
+      <c r="A122" s="71"/>
+      <c r="B122" s="58" t="s">
         <v>244</v>
       </c>
-      <c r="C122" s="60" t="s">
+      <c r="C122" s="59" t="s">
         <v>385</v>
       </c>
-      <c r="D122" s="59" t="s">
+      <c r="D122" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="E122" s="61"/>
-      <c r="F122" s="60"/>
+      <c r="E122" s="60"/>
+      <c r="F122" s="59"/>
     </row>
     <row r="123" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A123" s="72"/>
-      <c r="B123" s="59" t="s">
+      <c r="A123" s="71"/>
+      <c r="B123" s="58" t="s">
         <v>449</v>
       </c>
-      <c r="C123" s="60" t="s">
+      <c r="C123" s="59" t="s">
         <v>450</v>
       </c>
-      <c r="D123" s="59" t="s">
+      <c r="D123" s="58" t="s">
         <v>446</v>
       </c>
-      <c r="E123" s="61"/>
-      <c r="F123" s="59" t="s">
+      <c r="E123" s="60"/>
+      <c r="F123" s="58" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="124" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="A124" s="72"/>
-      <c r="B124" s="59" t="s">
+      <c r="A124" s="71"/>
+      <c r="B124" s="58" t="s">
         <v>246</v>
       </c>
-      <c r="C124" s="60" t="s">
+      <c r="C124" s="59" t="s">
         <v>386</v>
       </c>
-      <c r="D124" s="60" t="s">
+      <c r="D124" s="59" t="s">
         <v>345</v>
       </c>
-      <c r="E124" s="61"/>
-      <c r="F124" s="60"/>
+      <c r="E124" s="60"/>
+      <c r="F124" s="59"/>
     </row>
     <row r="125" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A125" s="72"/>
-      <c r="B125" s="59" t="s">
+      <c r="A125" s="71"/>
+      <c r="B125" s="58" t="s">
         <v>248</v>
       </c>
-      <c r="C125" s="60" t="s">
+      <c r="C125" s="59" t="s">
         <v>387</v>
       </c>
-      <c r="D125" s="60" t="s">
+      <c r="D125" s="59" t="s">
         <v>347</v>
       </c>
-      <c r="E125" s="61"/>
-      <c r="F125" s="60"/>
+      <c r="E125" s="60"/>
+      <c r="F125" s="59"/>
     </row>
     <row r="126" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A126" s="72"/>
-      <c r="B126" s="59" t="s">
+      <c r="A126" s="71"/>
+      <c r="B126" s="58" t="s">
         <v>250</v>
       </c>
-      <c r="C126" s="60" t="s">
+      <c r="C126" s="59" t="s">
         <v>388</v>
       </c>
-      <c r="D126" s="59" t="s">
+      <c r="D126" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="E126" s="61"/>
-      <c r="F126" s="60"/>
+      <c r="E126" s="60"/>
+      <c r="F126" s="59"/>
     </row>
     <row r="127" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A127" s="72"/>
-      <c r="B127" s="59" t="s">
+      <c r="A127" s="71"/>
+      <c r="B127" s="58" t="s">
         <v>453</v>
       </c>
-      <c r="C127" s="60" t="s">
+      <c r="C127" s="59" t="s">
         <v>454</v>
       </c>
-      <c r="D127" s="59" t="s">
+      <c r="D127" s="58" t="s">
         <v>550</v>
       </c>
-      <c r="E127" s="61"/>
-      <c r="F127" s="60" t="s">
+      <c r="E127" s="60"/>
+      <c r="F127" s="59" t="s">
         <v>464</v>
       </c>
     </row>
     <row r="128" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A128" s="72"/>
-      <c r="B128" s="59" t="s">
+      <c r="A128" s="71"/>
+      <c r="B128" s="58" t="s">
         <v>499</v>
       </c>
-      <c r="C128" s="60" t="s">
+      <c r="C128" s="59" t="s">
         <v>496</v>
       </c>
-      <c r="D128" s="60" t="s">
+      <c r="D128" s="59" t="s">
         <v>551</v>
       </c>
-      <c r="E128" s="61"/>
-      <c r="F128" s="60" t="s">
+      <c r="E128" s="60"/>
+      <c r="F128" s="59" t="s">
         <v>497</v>
       </c>
     </row>
     <row r="129" spans="1:6" ht="180" x14ac:dyDescent="0.25">
-      <c r="A129" s="72"/>
-      <c r="B129" s="59" t="s">
+      <c r="A129" s="71"/>
+      <c r="B129" s="58" t="s">
         <v>252</v>
       </c>
-      <c r="C129" s="60" t="s">
+      <c r="C129" s="59" t="s">
         <v>389</v>
       </c>
-      <c r="D129" s="60" t="s">
+      <c r="D129" s="59" t="s">
         <v>350</v>
       </c>
-      <c r="E129" s="61"/>
-      <c r="F129" s="60"/>
+      <c r="E129" s="60"/>
+      <c r="F129" s="59"/>
     </row>
     <row r="130" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A130" s="72"/>
-      <c r="B130" s="59" t="s">
+      <c r="A130" s="71"/>
+      <c r="B130" s="58" t="s">
         <v>254</v>
       </c>
-      <c r="C130" s="60" t="s">
+      <c r="C130" s="59" t="s">
         <v>390</v>
       </c>
-      <c r="D130" s="59" t="s">
+      <c r="D130" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E130" s="61"/>
-      <c r="F130" s="60"/>
+      <c r="E130" s="60"/>
+      <c r="F130" s="59"/>
     </row>
     <row r="131" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A131" s="72"/>
-      <c r="B131" s="59" t="s">
+      <c r="A131" s="71"/>
+      <c r="B131" s="58" t="s">
         <v>257</v>
       </c>
-      <c r="C131" s="60" t="s">
+      <c r="C131" s="59" t="s">
         <v>391</v>
       </c>
-      <c r="D131" s="60" t="s">
+      <c r="D131" s="59" t="s">
         <v>353</v>
       </c>
-      <c r="E131" s="61"/>
-      <c r="F131" s="60"/>
+      <c r="E131" s="60"/>
+      <c r="F131" s="59"/>
     </row>
     <row r="132" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A132" s="72"/>
-      <c r="B132" s="59" t="s">
+      <c r="A132" s="71"/>
+      <c r="B132" s="58" t="s">
         <v>259</v>
       </c>
-      <c r="C132" s="60" t="s">
+      <c r="C132" s="59" t="s">
         <v>392</v>
       </c>
-      <c r="D132" s="59" t="s">
+      <c r="D132" s="58" t="s">
         <v>261</v>
       </c>
-      <c r="E132" s="61"/>
-      <c r="F132" s="60"/>
+      <c r="E132" s="60"/>
+      <c r="F132" s="59"/>
     </row>
     <row r="133" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A133" s="72"/>
-      <c r="B133" s="59" t="s">
+      <c r="A133" s="71"/>
+      <c r="B133" s="58" t="s">
         <v>262</v>
       </c>
-      <c r="C133" s="60" t="s">
+      <c r="C133" s="59" t="s">
         <v>393</v>
       </c>
-      <c r="D133" s="59" t="s">
+      <c r="D133" s="58" t="s">
         <v>261</v>
       </c>
-      <c r="E133" s="61"/>
-      <c r="F133" s="60"/>
+      <c r="E133" s="60"/>
+      <c r="F133" s="59"/>
     </row>
     <row r="134" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A134" s="72"/>
-      <c r="B134" s="59" t="s">
+      <c r="A134" s="71"/>
+      <c r="B134" s="58" t="s">
         <v>264</v>
       </c>
-      <c r="C134" s="60" t="s">
+      <c r="C134" s="59" t="s">
         <v>394</v>
       </c>
-      <c r="D134" s="59" t="s">
+      <c r="D134" s="58" t="s">
         <v>261</v>
       </c>
-      <c r="E134" s="61"/>
-      <c r="F134" s="60"/>
+      <c r="E134" s="60"/>
+      <c r="F134" s="59"/>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A135" s="72"/>
-      <c r="B135" s="59" t="s">
+      <c r="A135" s="71"/>
+      <c r="B135" s="58" t="s">
         <v>266</v>
       </c>
-      <c r="C135" s="59" t="s">
+      <c r="C135" s="58" t="s">
         <v>267</v>
       </c>
-      <c r="D135" s="59" t="s">
+      <c r="D135" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="E135" s="61"/>
-      <c r="F135" s="60"/>
+      <c r="E135" s="60"/>
+      <c r="F135" s="59"/>
     </row>
     <row r="136" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A136" s="72"/>
-      <c r="B136" s="59" t="s">
+      <c r="A136" s="71"/>
+      <c r="B136" s="58" t="s">
         <v>268</v>
       </c>
-      <c r="C136" s="60" t="s">
+      <c r="C136" s="59" t="s">
         <v>395</v>
       </c>
-      <c r="D136" s="59" t="s">
+      <c r="D136" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="E136" s="61"/>
-      <c r="F136" s="60"/>
+      <c r="E136" s="60"/>
+      <c r="F136" s="59"/>
     </row>
     <row r="137" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A137" s="72"/>
-      <c r="B137" s="59" t="s">
+      <c r="A137" s="71"/>
+      <c r="B137" s="58" t="s">
         <v>270</v>
       </c>
-      <c r="C137" s="60" t="s">
+      <c r="C137" s="59" t="s">
         <v>396</v>
       </c>
-      <c r="D137" s="59" t="s">
+      <c r="D137" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="E137" s="61"/>
-      <c r="F137" s="60"/>
+      <c r="E137" s="60"/>
+      <c r="F137" s="59"/>
     </row>
     <row r="138" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A138" s="72"/>
-      <c r="B138" s="59" t="s">
+      <c r="A138" s="71"/>
+      <c r="B138" s="58" t="s">
         <v>272</v>
       </c>
-      <c r="C138" s="60" t="s">
+      <c r="C138" s="59" t="s">
         <v>397</v>
       </c>
-      <c r="D138" s="59" t="s">
+      <c r="D138" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="E138" s="61"/>
-      <c r="F138" s="60"/>
+      <c r="E138" s="60"/>
+      <c r="F138" s="59"/>
     </row>
     <row r="139" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A139" s="72"/>
-      <c r="B139" s="59" t="s">
+      <c r="A139" s="71"/>
+      <c r="B139" s="58" t="s">
         <v>274</v>
       </c>
-      <c r="C139" s="60" t="s">
+      <c r="C139" s="59" t="s">
         <v>398</v>
       </c>
-      <c r="D139" s="59" t="s">
+      <c r="D139" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E139" s="61"/>
-      <c r="F139" s="60"/>
+      <c r="E139" s="60"/>
+      <c r="F139" s="59"/>
     </row>
     <row r="140" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A140" s="72"/>
-      <c r="B140" s="59" t="s">
+      <c r="A140" s="71"/>
+      <c r="B140" s="58" t="s">
         <v>276</v>
       </c>
-      <c r="C140" s="60" t="s">
+      <c r="C140" s="59" t="s">
         <v>399</v>
       </c>
-      <c r="D140" s="59" t="s">
+      <c r="D140" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E140" s="61"/>
-      <c r="F140" s="60"/>
+      <c r="E140" s="60"/>
+      <c r="F140" s="59"/>
     </row>
     <row r="141" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A141" s="72"/>
-      <c r="B141" s="59" t="s">
+      <c r="A141" s="71"/>
+      <c r="B141" s="58" t="s">
         <v>278</v>
       </c>
-      <c r="C141" s="60" t="s">
+      <c r="C141" s="59" t="s">
         <v>400</v>
       </c>
-      <c r="D141" s="60" t="s">
+      <c r="D141" s="59" t="s">
         <v>340</v>
       </c>
-      <c r="E141" s="61" t="s">
+      <c r="E141" s="60" t="s">
         <v>278</v>
       </c>
-      <c r="F141" s="60"/>
+      <c r="F141" s="59"/>
     </row>
     <row r="142" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A142" s="72"/>
-      <c r="B142" s="59" t="s">
+      <c r="A142" s="71"/>
+      <c r="B142" s="58" t="s">
         <v>280</v>
       </c>
-      <c r="C142" s="60" t="s">
+      <c r="C142" s="59" t="s">
         <v>401</v>
       </c>
-      <c r="D142" s="60" t="s">
+      <c r="D142" s="59" t="s">
         <v>342</v>
       </c>
-      <c r="E142" s="61"/>
-      <c r="F142" s="60"/>
+      <c r="E142" s="60"/>
+      <c r="F142" s="59"/>
     </row>
     <row r="143" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A143" s="72"/>
-      <c r="B143" s="59" t="s">
+      <c r="A143" s="71"/>
+      <c r="B143" s="58" t="s">
         <v>471</v>
       </c>
-      <c r="C143" s="60" t="s">
+      <c r="C143" s="59" t="s">
         <v>402</v>
       </c>
-      <c r="D143" s="59" t="s">
+      <c r="D143" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="E143" s="61"/>
-      <c r="F143" s="60"/>
+      <c r="E143" s="60"/>
+      <c r="F143" s="59"/>
     </row>
     <row r="144" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A144" s="72"/>
-      <c r="B144" s="59" t="s">
+      <c r="A144" s="71"/>
+      <c r="B144" s="58" t="s">
         <v>455</v>
       </c>
-      <c r="C144" s="60" t="s">
+      <c r="C144" s="59" t="s">
         <v>456</v>
       </c>
-      <c r="D144" s="59" t="s">
+      <c r="D144" s="58" t="s">
         <v>446</v>
       </c>
-      <c r="E144" s="61"/>
-      <c r="F144" s="59" t="s">
+      <c r="E144" s="60"/>
+      <c r="F144" s="58" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="145" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="A145" s="72"/>
-      <c r="B145" s="59" t="s">
+      <c r="A145" s="71"/>
+      <c r="B145" s="58" t="s">
         <v>284</v>
       </c>
-      <c r="C145" s="60" t="s">
+      <c r="C145" s="59" t="s">
         <v>403</v>
       </c>
-      <c r="D145" s="60" t="s">
+      <c r="D145" s="59" t="s">
         <v>345</v>
       </c>
-      <c r="E145" s="61"/>
-      <c r="F145" s="60"/>
+      <c r="E145" s="60"/>
+      <c r="F145" s="59"/>
     </row>
     <row r="146" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A146" s="72"/>
-      <c r="B146" s="59" t="s">
+      <c r="A146" s="71"/>
+      <c r="B146" s="58" t="s">
         <v>287</v>
       </c>
-      <c r="C146" s="60" t="s">
+      <c r="C146" s="59" t="s">
         <v>404</v>
       </c>
-      <c r="D146" s="60" t="s">
+      <c r="D146" s="59" t="s">
         <v>347</v>
       </c>
-      <c r="E146" s="61"/>
-      <c r="F146" s="60"/>
+      <c r="E146" s="60"/>
+      <c r="F146" s="59"/>
     </row>
     <row r="147" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A147" s="72"/>
-      <c r="B147" s="59" t="s">
+      <c r="A147" s="71"/>
+      <c r="B147" s="58" t="s">
         <v>289</v>
       </c>
-      <c r="C147" s="60" t="s">
+      <c r="C147" s="59" t="s">
         <v>290</v>
       </c>
-      <c r="D147" s="59" t="s">
+      <c r="D147" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="E147" s="61"/>
-      <c r="F147" s="60"/>
+      <c r="E147" s="60"/>
+      <c r="F147" s="59"/>
     </row>
     <row r="148" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A148" s="72"/>
-      <c r="B148" s="59" t="s">
+      <c r="A148" s="71"/>
+      <c r="B148" s="58" t="s">
         <v>457</v>
       </c>
-      <c r="C148" s="60" t="s">
+      <c r="C148" s="59" t="s">
         <v>458</v>
       </c>
-      <c r="D148" s="59" t="s">
+      <c r="D148" s="58" t="s">
         <v>550</v>
       </c>
-      <c r="E148" s="61"/>
-      <c r="F148" s="60" t="s">
+      <c r="E148" s="60"/>
+      <c r="F148" s="59" t="s">
         <v>464</v>
       </c>
     </row>
     <row r="149" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A149" s="72"/>
-      <c r="B149" s="59" t="s">
+      <c r="A149" s="71"/>
+      <c r="B149" s="58" t="s">
         <v>500</v>
       </c>
-      <c r="C149" s="60" t="s">
+      <c r="C149" s="59" t="s">
         <v>496</v>
       </c>
-      <c r="D149" s="60" t="s">
+      <c r="D149" s="59" t="s">
         <v>551</v>
       </c>
-      <c r="E149" s="61"/>
-      <c r="F149" s="60" t="s">
+      <c r="E149" s="60"/>
+      <c r="F149" s="59" t="s">
         <v>497</v>
       </c>
     </row>
     <row r="150" spans="1:6" ht="180" x14ac:dyDescent="0.25">
-      <c r="A150" s="72"/>
-      <c r="B150" s="59" t="s">
+      <c r="A150" s="71"/>
+      <c r="B150" s="58" t="s">
         <v>291</v>
       </c>
-      <c r="C150" s="60" t="s">
+      <c r="C150" s="59" t="s">
         <v>405</v>
       </c>
-      <c r="D150" s="60" t="s">
+      <c r="D150" s="59" t="s">
         <v>350</v>
       </c>
-      <c r="E150" s="61"/>
-      <c r="F150" s="60"/>
+      <c r="E150" s="60"/>
+      <c r="F150" s="59"/>
     </row>
     <row r="151" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A151" s="72"/>
-      <c r="B151" s="59" t="s">
+      <c r="A151" s="71"/>
+      <c r="B151" s="58" t="s">
         <v>293</v>
       </c>
-      <c r="C151" s="60" t="s">
+      <c r="C151" s="59" t="s">
         <v>406</v>
       </c>
-      <c r="D151" s="59" t="s">
+      <c r="D151" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E151" s="61"/>
-      <c r="F151" s="60"/>
+      <c r="E151" s="60"/>
+      <c r="F151" s="59"/>
     </row>
     <row r="152" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A152" s="72"/>
-      <c r="B152" s="59" t="s">
+      <c r="A152" s="71"/>
+      <c r="B152" s="58" t="s">
         <v>296</v>
       </c>
-      <c r="C152" s="60" t="s">
+      <c r="C152" s="59" t="s">
         <v>407</v>
       </c>
-      <c r="D152" s="60" t="s">
+      <c r="D152" s="59" t="s">
         <v>353</v>
       </c>
-      <c r="E152" s="61"/>
-      <c r="F152" s="60"/>
+      <c r="E152" s="60"/>
+      <c r="F152" s="59"/>
     </row>
     <row r="153" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A153" s="72"/>
-      <c r="B153" s="59" t="s">
+      <c r="A153" s="71"/>
+      <c r="B153" s="58" t="s">
         <v>298</v>
       </c>
-      <c r="C153" s="60" t="s">
+      <c r="C153" s="59" t="s">
         <v>408</v>
       </c>
-      <c r="D153" s="59" t="s">
+      <c r="D153" s="58" t="s">
         <v>300</v>
       </c>
-      <c r="E153" s="61"/>
-      <c r="F153" s="60"/>
+      <c r="E153" s="60"/>
+      <c r="F153" s="59"/>
     </row>
     <row r="154" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A154" s="72"/>
-      <c r="B154" s="59" t="s">
+      <c r="A154" s="71"/>
+      <c r="B154" s="58" t="s">
         <v>301</v>
       </c>
-      <c r="C154" s="60" t="s">
+      <c r="C154" s="59" t="s">
         <v>409</v>
       </c>
-      <c r="D154" s="59" t="s">
+      <c r="D154" s="58" t="s">
         <v>261</v>
       </c>
-      <c r="E154" s="61"/>
-      <c r="F154" s="60"/>
+      <c r="E154" s="60"/>
+      <c r="F154" s="59"/>
     </row>
     <row r="155" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A155" s="72"/>
-      <c r="B155" s="59" t="s">
+      <c r="A155" s="71"/>
+      <c r="B155" s="58" t="s">
         <v>303</v>
       </c>
-      <c r="C155" s="60" t="s">
+      <c r="C155" s="59" t="s">
         <v>410</v>
       </c>
-      <c r="D155" s="59"/>
-      <c r="E155" s="61"/>
-      <c r="F155" s="60"/>
+      <c r="D155" s="58"/>
+      <c r="E155" s="60"/>
+      <c r="F155" s="59"/>
     </row>
     <row r="156" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A156" s="72"/>
-      <c r="B156" s="59" t="s">
+      <c r="A156" s="71"/>
+      <c r="B156" s="58" t="s">
         <v>305</v>
       </c>
-      <c r="C156" s="60" t="s">
+      <c r="C156" s="59" t="s">
         <v>411</v>
       </c>
-      <c r="D156" s="59" t="s">
+      <c r="D156" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E156" s="61"/>
-      <c r="F156" s="60"/>
+      <c r="E156" s="60"/>
+      <c r="F156" s="59"/>
     </row>
     <row r="157" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A157" s="72"/>
-      <c r="B157" s="59" t="s">
+      <c r="A157" s="71"/>
+      <c r="B157" s="58" t="s">
         <v>307</v>
       </c>
-      <c r="C157" s="60" t="s">
+      <c r="C157" s="59" t="s">
         <v>412</v>
       </c>
-      <c r="D157" s="59" t="s">
+      <c r="D157" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E157" s="61"/>
-      <c r="F157" s="60"/>
+      <c r="E157" s="60"/>
+      <c r="F157" s="59"/>
     </row>
     <row r="158" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A158" s="72"/>
-      <c r="B158" s="59" t="s">
+      <c r="A158" s="71"/>
+      <c r="B158" s="58" t="s">
         <v>309</v>
       </c>
-      <c r="C158" s="60" t="s">
+      <c r="C158" s="59" t="s">
         <v>413</v>
       </c>
-      <c r="D158" s="59" t="s">
+      <c r="D158" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E158" s="61"/>
-      <c r="F158" s="60"/>
+      <c r="E158" s="60"/>
+      <c r="F158" s="59"/>
     </row>
     <row r="159" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A159" s="72"/>
-      <c r="B159" s="59" t="s">
+      <c r="A159" s="71"/>
+      <c r="B159" s="58" t="s">
         <v>311</v>
       </c>
-      <c r="C159" s="60" t="s">
+      <c r="C159" s="59" t="s">
         <v>414</v>
       </c>
-      <c r="D159" s="59" t="s">
+      <c r="D159" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E159" s="61"/>
-      <c r="F159" s="60"/>
+      <c r="E159" s="60"/>
+      <c r="F159" s="59"/>
     </row>
     <row r="160" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A160" s="72"/>
-      <c r="B160" s="59" t="s">
+      <c r="A160" s="71"/>
+      <c r="B160" s="58" t="s">
         <v>224</v>
       </c>
-      <c r="C160" s="60" t="s">
+      <c r="C160" s="59" t="s">
         <v>415</v>
       </c>
-      <c r="D160" s="59" t="s">
+      <c r="D160" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E160" s="61"/>
-      <c r="F160" s="60"/>
+      <c r="E160" s="60"/>
+      <c r="F160" s="59"/>
     </row>
     <row r="161" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A161" s="72"/>
-      <c r="B161" s="59" t="s">
+      <c r="A161" s="71"/>
+      <c r="B161" s="58" t="s">
         <v>315</v>
       </c>
-      <c r="C161" s="60" t="s">
+      <c r="C161" s="59" t="s">
         <v>416</v>
       </c>
-      <c r="D161" s="59" t="s">
+      <c r="D161" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E161" s="61"/>
-      <c r="F161" s="60"/>
+      <c r="E161" s="60"/>
+      <c r="F161" s="59"/>
     </row>
     <row r="162" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A162" s="72"/>
-      <c r="B162" s="59" t="s">
+      <c r="A162" s="71"/>
+      <c r="B162" s="58" t="s">
         <v>317</v>
       </c>
-      <c r="C162" s="60" t="s">
+      <c r="C162" s="59" t="s">
         <v>417</v>
       </c>
-      <c r="D162" s="59" t="s">
+      <c r="D162" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E162" s="61"/>
-      <c r="F162" s="60"/>
+      <c r="E162" s="60"/>
+      <c r="F162" s="59"/>
     </row>
     <row r="163" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A163" s="72"/>
-      <c r="B163" s="59" t="s">
+      <c r="A163" s="71"/>
+      <c r="B163" s="58" t="s">
         <v>319</v>
       </c>
-      <c r="C163" s="60" t="s">
+      <c r="C163" s="59" t="s">
         <v>418</v>
       </c>
-      <c r="D163" s="59" t="s">
+      <c r="D163" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E163" s="61"/>
-      <c r="F163" s="60"/>
+      <c r="E163" s="60"/>
+      <c r="F163" s="59"/>
     </row>
     <row r="164" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="A164" s="72"/>
-      <c r="B164" s="59" t="s">
+      <c r="A164" s="71"/>
+      <c r="B164" s="58" t="s">
         <v>321</v>
       </c>
-      <c r="C164" s="59" t="s">
+      <c r="C164" s="58" t="s">
         <v>322</v>
       </c>
-      <c r="D164" s="59" t="s">
+      <c r="D164" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E164" s="61" t="s">
+      <c r="E164" s="60" t="s">
         <v>321</v>
       </c>
-      <c r="F164" s="60" t="s">
+      <c r="F164" s="59" t="s">
         <v>419</v>
       </c>
     </row>
     <row r="165" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A165" s="72"/>
-      <c r="B165" s="59"/>
-      <c r="C165" s="59"/>
-      <c r="D165" s="59"/>
-      <c r="E165" s="61" t="s">
+      <c r="A165" s="71"/>
+      <c r="B165" s="58"/>
+      <c r="C165" s="58"/>
+      <c r="D165" s="58"/>
+      <c r="E165" s="60" t="s">
         <v>323</v>
       </c>
-      <c r="F165" s="60" t="s">
+      <c r="F165" s="59" t="s">
         <v>420</v>
       </c>
     </row>
     <row r="166" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A166" s="72"/>
-      <c r="B166" s="59" t="s">
+      <c r="A166" s="71"/>
+      <c r="B166" s="58" t="s">
         <v>324</v>
       </c>
-      <c r="C166" s="60" t="s">
+      <c r="C166" s="59" t="s">
         <v>425</v>
       </c>
-      <c r="D166" s="59" t="s">
+      <c r="D166" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E166" s="61"/>
-      <c r="F166" s="60"/>
+      <c r="E166" s="60"/>
+      <c r="F166" s="59"/>
     </row>
     <row r="167" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A167" s="72"/>
-      <c r="B167" s="59" t="s">
+      <c r="A167" s="71"/>
+      <c r="B167" s="58" t="s">
         <v>326</v>
       </c>
-      <c r="C167" s="60" t="s">
+      <c r="C167" s="59" t="s">
         <v>426</v>
       </c>
-      <c r="D167" s="59" t="s">
+      <c r="D167" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E167" s="61"/>
-      <c r="F167" s="60" t="s">
+      <c r="E167" s="60"/>
+      <c r="F167" s="59" t="s">
         <v>429</v>
       </c>
     </row>
     <row r="168" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A168" s="72"/>
-      <c r="B168" s="62" t="s">
+      <c r="A168" s="71"/>
+      <c r="B168" s="61" t="s">
         <v>328</v>
       </c>
-      <c r="C168" s="63" t="s">
+      <c r="C168" s="62" t="s">
         <v>427</v>
       </c>
-      <c r="D168" s="62" t="s">
+      <c r="D168" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="E168" s="64"/>
-      <c r="F168" s="63" t="s">
+      <c r="E168" s="63"/>
+      <c r="F168" s="62" t="s">
         <v>428</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F168" xr:uid="{EA55B166-B49F-4ECB-9A75-5F440FA2BF9F}"/>
   <mergeCells count="8">
-    <mergeCell ref="A2:A19"/>
+    <mergeCell ref="A2:A20"/>
     <mergeCell ref="A63:A168"/>
-    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="A21:A26"/>
     <mergeCell ref="F33:F38"/>
     <mergeCell ref="A27:A38"/>
     <mergeCell ref="A39:A47"/>
@@ -7855,53 +7877,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="2a6c10d7-b926-4fc0-945e-3cbf5049f6bd" ContentTypeId="0x010100F4C63C3BD852AE468EAEFD0E6C57C64F02" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events"/>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <o1cb080a3dca4eb8a0fd03c7cc8bf8f7 xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </o1cb080a3dca4eb8a0fd03c7cc8bf8f7>
-    <Abstract xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d" xsi:nil="true"/>
-    <WBDocs_Access_To_Info_Exception xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">12. Not Assessed</WBDocs_Access_To_Info_Exception>
-    <WBDocs_Document_Date xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">2020-12-22T17:31:22+00:00</WBDocs_Document_Date>
-    <TaxCatchAll xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">
-      <Value>5</Value>
-      <Value>3</Value>
-    </TaxCatchAll>
-    <OneCMS_Subcategory xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d" xsi:nil="true"/>
-    <i008215bacac45029ee8cafff4c8e93b xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">HSJDR</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">b82b4e50-8b87-486b-adae-4a5ffb2d1593</TermId>
-        </TermInfo>
-      </Terms>
-    </i008215bacac45029ee8cafff4c8e93b>
-    <WBDocs_Information_Classification xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">Official Use Only</WBDocs_Information_Classification>
-    <OneCMS_Category xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="WBDocument" ma:contentTypeID="0x010100F4C63C3BD852AE468EAEFD0E6C57C64F020023FF955149D2434D9634B069E3D44A42" ma:contentTypeVersion="49" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="765f642684fa63bc1b9312c368d0b6a5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3e02667f-0271-471b-bd6e-11a2e16def1d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e953fe045711556fedbcbd575ad79d22" ns3:_="">
     <xsd:import namespace="3e02667f-0271-471b-bd6e-11a2e16def1d"/>
@@ -8143,31 +8118,72 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <o1cb080a3dca4eb8a0fd03c7cc8bf8f7 xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </o1cb080a3dca4eb8a0fd03c7cc8bf8f7>
+    <Abstract xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d" xsi:nil="true"/>
+    <WBDocs_Access_To_Info_Exception xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">12. Not Assessed</WBDocs_Access_To_Info_Exception>
+    <WBDocs_Document_Date xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">2020-12-22T17:31:22+00:00</WBDocs_Document_Date>
+    <TaxCatchAll xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">
+      <Value>5</Value>
+      <Value>3</Value>
+    </TaxCatchAll>
+    <OneCMS_Subcategory xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d" xsi:nil="true"/>
+    <i008215bacac45029ee8cafff4c8e93b xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">HSJDR</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">b82b4e50-8b87-486b-adae-4a5ffb2d1593</TermId>
+        </TermInfo>
+      </Terms>
+    </i008215bacac45029ee8cafff4c8e93b>
+    <WBDocs_Information_Classification xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">Official Use Only</WBDocs_Information_Classification>
+    <OneCMS_Category xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events"/>
+</file>
+
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="2a6c10d7-b926-4fc0-945e-3cbf5049f6bd" ContentTypeId="0x010100F4C63C3BD852AE468EAEFD0E6C57C64F02" PreviousValue="false"/>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60C49A35-6CF8-4B2E-BB80-5700FA61EE99}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA715D2A-5893-441B-82FC-527C371B80FF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3e02667f-0271-471b-bd6e-11a2e16def1d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B32DBFF-5393-4654-88B0-C956207D28B5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8074832C-F0BA-4806-8675-5DC290219507}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33B6C801-2D56-49AD-B646-66F2DEE67E6F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -8183,20 +8199,26 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8074832C-F0BA-4806-8675-5DC290219507}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B32DBFF-5393-4654-88B0-C956207D28B5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA715D2A-5893-441B-82FC-527C371B80FF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60C49A35-6CF8-4B2E-BB80-5700FA61EE99}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3e02667f-0271-471b-bd6e-11a2e16def1d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>